<commit_message>
cambios a flujos transaccionales y nuevo correo
</commit_message>
<xml_diff>
--- a/data/FlujosTransaccionales.xlsx
+++ b/data/FlujosTransaccionales.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atcon\Desktop\Playwright\playwright-piloto2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D20BC2CF-A202-4834-965A-3E83270EA74E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A965DB8-9DFF-4759-8F74-A3DD026FB270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{522E3CD9-5E7D-4978-84C2-A91ECF51BF07}"/>
   </bookViews>
@@ -45,6 +45,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Matriz modificada  24 Junio 24'!$A$1:$M$33</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3860" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3859" uniqueCount="401">
   <si>
     <t>ID</t>
   </si>
@@ -1506,7 +1507,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1677,12 +1678,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF272626"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="19">
@@ -2132,7 +2127,7 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2475,6 +2470,56 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="13" fillId="14" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="13" fillId="14" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2508,57 +2553,6 @@
     <xf numFmtId="0" fontId="15" fillId="14" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="13" fillId="14" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="13" fillId="14" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -2941,7 +2935,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7432F683-F664-4C95-88E4-2A9AFFFC0E8D}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -2962,7 +2956,7 @@
       <c r="B1" t="s">
         <v>390</v>
       </c>
-      <c r="C1" s="143" t="s">
+      <c r="C1" s="116" t="s">
         <v>393</v>
       </c>
       <c r="D1" t="s">
@@ -2994,25 +2988,25 @@
       <c r="B2" t="s">
         <v>383</v>
       </c>
-      <c r="C2" s="144"/>
+      <c r="C2" s="117"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>384</v>
       </c>
       <c r="B3" t="s">
-        <v>385</v>
-      </c>
-      <c r="C3" s="144"/>
+        <v>384</v>
+      </c>
+      <c r="C3" s="117"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>385</v>
       </c>
       <c r="B4" t="s">
-        <v>384</v>
-      </c>
-      <c r="C4" s="144">
+        <v>385</v>
+      </c>
+      <c r="C4" s="117">
         <v>4111111111111110</v>
       </c>
       <c r="I4" t="s">
@@ -3024,9 +3018,9 @@
         <v>386</v>
       </c>
       <c r="B5" t="s">
-        <v>384</v>
-      </c>
-      <c r="C5" s="144">
+        <v>386</v>
+      </c>
+      <c r="C5" s="117">
         <v>5105105105105100</v>
       </c>
       <c r="I5" t="s">
@@ -3038,82 +3032,18 @@
         <v>387</v>
       </c>
       <c r="B6" t="s">
-        <v>386</v>
-      </c>
-      <c r="C6" s="144"/>
+        <v>387</v>
+      </c>
+      <c r="C6" s="117"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>388</v>
       </c>
       <c r="B7" t="s">
-        <v>387</v>
-      </c>
-      <c r="C7" s="144"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="B8" t="s">
         <v>388</v>
       </c>
-      <c r="C8" s="144"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="C9" s="144"/>
-      <c r="J9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="C10" s="144"/>
-      <c r="F10" s="143"/>
-      <c r="J10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="C11" s="144"/>
-      <c r="J11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="C12" s="144"/>
-      <c r="J12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="C13" s="145"/>
-      <c r="J13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="C14" s="144"/>
-      <c r="J14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="C15" s="144"/>
-      <c r="J15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="C16" s="144"/>
-      <c r="J16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="3:10">
-      <c r="C17" s="144"/>
-      <c r="J17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="3:10">
-      <c r="C18" s="144"/>
+      <c r="C7" s="117"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10697,28 +10627,28 @@
     </row>
     <row r="3" spans="1:31" ht="15.75" customHeight="1">
       <c r="B3" s="44"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="116"/>
-      <c r="G3" s="116"/>
-      <c r="H3" s="116"/>
-      <c r="I3" s="116"/>
-      <c r="J3" s="116"/>
-      <c r="K3" s="116"/>
-      <c r="L3" s="116"/>
-      <c r="M3" s="116"/>
-      <c r="N3" s="116"/>
-      <c r="O3" s="116"/>
-      <c r="P3" s="116"/>
-      <c r="Q3" s="116"/>
-      <c r="R3" s="116"/>
-      <c r="S3" s="116"/>
+      <c r="C3" s="134"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
+      <c r="H3" s="134"/>
+      <c r="I3" s="134"/>
+      <c r="J3" s="134"/>
+      <c r="K3" s="134"/>
+      <c r="L3" s="134"/>
+      <c r="M3" s="134"/>
+      <c r="N3" s="134"/>
+      <c r="O3" s="134"/>
+      <c r="P3" s="134"/>
+      <c r="Q3" s="134"/>
+      <c r="R3" s="134"/>
+      <c r="S3" s="134"/>
       <c r="T3" s="45"/>
-      <c r="Y3" s="117"/>
-      <c r="Z3" s="117"/>
-      <c r="AA3" s="117"/>
-      <c r="AB3" s="117"/>
+      <c r="Y3" s="135"/>
+      <c r="Z3" s="135"/>
+      <c r="AA3" s="135"/>
+      <c r="AB3" s="135"/>
     </row>
     <row r="4" spans="1:31" ht="15" customHeight="1">
       <c r="B4" s="44"/>
@@ -10743,47 +10673,47 @@
     </row>
     <row r="5" spans="1:31" s="49" customFormat="1" ht="12.75" customHeight="1">
       <c r="B5" s="50"/>
-      <c r="C5" s="118" t="s">
+      <c r="C5" s="136" t="s">
         <v>358</v>
       </c>
-      <c r="D5" s="119"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="127" t="s">
+      <c r="D5" s="137"/>
+      <c r="E5" s="138"/>
+      <c r="F5" s="118" t="s">
         <v>359</v>
       </c>
-      <c r="G5" s="127" t="s">
+      <c r="G5" s="118" t="s">
         <v>360</v>
       </c>
-      <c r="H5" s="127" t="s">
+      <c r="H5" s="118" t="s">
         <v>361</v>
       </c>
-      <c r="I5" s="127" t="s">
+      <c r="I5" s="118" t="s">
         <v>362</v>
       </c>
-      <c r="J5" s="127" t="s">
+      <c r="J5" s="118" t="s">
         <v>363</v>
       </c>
-      <c r="K5" s="127" t="s">
+      <c r="K5" s="118" t="s">
         <v>364</v>
       </c>
-      <c r="L5" s="127" t="s">
+      <c r="L5" s="118" t="s">
         <v>365</v>
       </c>
-      <c r="M5" s="129" t="s">
+      <c r="M5" s="126" t="s">
         <v>366</v>
       </c>
-      <c r="N5" s="129" t="s">
+      <c r="N5" s="126" t="s">
         <v>367</v>
       </c>
-      <c r="O5" s="129" t="s">
+      <c r="O5" s="126" t="s">
         <v>368</v>
       </c>
-      <c r="P5" s="131" t="s">
+      <c r="P5" s="120" t="s">
         <v>369</v>
       </c>
-      <c r="Q5" s="132"/>
-      <c r="R5" s="132"/>
-      <c r="S5" s="133"/>
+      <c r="Q5" s="121"/>
+      <c r="R5" s="121"/>
+      <c r="S5" s="122"/>
       <c r="T5" s="51"/>
       <c r="U5" s="52"/>
       <c r="Y5" s="53"/>
@@ -10796,19 +10726,19 @@
     </row>
     <row r="6" spans="1:31" s="49" customFormat="1" ht="15" customHeight="1">
       <c r="B6" s="50"/>
-      <c r="C6" s="121"/>
-      <c r="D6" s="122"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="128"/>
-      <c r="H6" s="128"/>
-      <c r="I6" s="128"/>
-      <c r="J6" s="128"/>
-      <c r="K6" s="128"/>
-      <c r="L6" s="128"/>
-      <c r="M6" s="130"/>
-      <c r="N6" s="130"/>
-      <c r="O6" s="130"/>
+      <c r="C6" s="139"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="141"/>
+      <c r="F6" s="119"/>
+      <c r="G6" s="119"/>
+      <c r="H6" s="119"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="119"/>
+      <c r="K6" s="119"/>
+      <c r="L6" s="119"/>
+      <c r="M6" s="127"/>
+      <c r="N6" s="127"/>
+      <c r="O6" s="127"/>
       <c r="P6" s="54" t="s">
         <v>370</v>
       </c>
@@ -10833,9 +10763,9 @@
     </row>
     <row r="7" spans="1:31" s="56" customFormat="1" ht="15.75" customHeight="1">
       <c r="B7" s="57"/>
-      <c r="C7" s="124"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="126"/>
+      <c r="C7" s="142"/>
+      <c r="D7" s="143"/>
+      <c r="E7" s="144"/>
       <c r="F7" s="58">
         <f>F14</f>
         <v>32</v>
@@ -10946,49 +10876,49 @@
     </row>
     <row r="9" spans="1:31" s="49" customFormat="1" ht="15" customHeight="1">
       <c r="B9" s="50"/>
-      <c r="C9" s="134" t="s">
+      <c r="C9" s="128" t="s">
         <v>374</v>
       </c>
-      <c r="D9" s="136" t="s">
+      <c r="D9" s="130" t="s">
         <v>375</v>
       </c>
-      <c r="E9" s="137"/>
-      <c r="F9" s="138" t="s">
+      <c r="E9" s="131"/>
+      <c r="F9" s="132" t="s">
         <v>359</v>
       </c>
-      <c r="G9" s="127" t="s">
+      <c r="G9" s="118" t="s">
         <v>360</v>
       </c>
-      <c r="H9" s="127" t="s">
+      <c r="H9" s="118" t="s">
         <v>361</v>
       </c>
-      <c r="I9" s="127" t="s">
+      <c r="I9" s="118" t="s">
         <v>362</v>
       </c>
-      <c r="J9" s="127" t="s">
+      <c r="J9" s="118" t="s">
         <v>363</v>
       </c>
-      <c r="K9" s="127" t="s">
+      <c r="K9" s="118" t="s">
         <v>376</v>
       </c>
-      <c r="L9" s="127" t="s">
+      <c r="L9" s="118" t="s">
         <v>365</v>
       </c>
-      <c r="M9" s="129" t="s">
+      <c r="M9" s="126" t="s">
         <v>366</v>
       </c>
-      <c r="N9" s="129" t="s">
+      <c r="N9" s="126" t="s">
         <v>367</v>
       </c>
-      <c r="O9" s="129" t="s">
+      <c r="O9" s="126" t="s">
         <v>368</v>
       </c>
-      <c r="P9" s="131" t="s">
+      <c r="P9" s="120" t="s">
         <v>369</v>
       </c>
-      <c r="Q9" s="132"/>
-      <c r="R9" s="132"/>
-      <c r="S9" s="133"/>
+      <c r="Q9" s="121"/>
+      <c r="R9" s="121"/>
+      <c r="S9" s="122"/>
       <c r="T9" s="67"/>
       <c r="U9" s="68"/>
       <c r="Y9" s="55"/>
@@ -11001,23 +10931,23 @@
     </row>
     <row r="10" spans="1:31" s="49" customFormat="1" ht="15" customHeight="1">
       <c r="B10" s="50"/>
-      <c r="C10" s="135"/>
+      <c r="C10" s="129"/>
       <c r="D10" s="69" t="s">
         <v>377</v>
       </c>
       <c r="E10" s="70" t="s">
         <v>378</v>
       </c>
-      <c r="F10" s="139"/>
-      <c r="G10" s="128"/>
-      <c r="H10" s="128"/>
-      <c r="I10" s="128"/>
-      <c r="J10" s="128"/>
-      <c r="K10" s="128"/>
-      <c r="L10" s="128"/>
-      <c r="M10" s="130"/>
-      <c r="N10" s="130"/>
-      <c r="O10" s="130"/>
+      <c r="F10" s="133"/>
+      <c r="G10" s="119"/>
+      <c r="H10" s="119"/>
+      <c r="I10" s="119"/>
+      <c r="J10" s="119"/>
+      <c r="K10" s="119"/>
+      <c r="L10" s="119"/>
+      <c r="M10" s="127"/>
+      <c r="N10" s="127"/>
+      <c r="O10" s="127"/>
       <c r="P10" s="54" t="s">
         <v>370</v>
       </c>
@@ -11045,10 +10975,10 @@
       <c r="C11" s="71" t="s">
         <v>379</v>
       </c>
-      <c r="D11" s="140" t="s">
+      <c r="D11" s="123" t="s">
         <v>380</v>
       </c>
-      <c r="E11" s="140"/>
+      <c r="E11" s="123"/>
       <c r="F11" s="73">
         <f t="shared" ref="F11:L11" si="3">SUM(F12:F13)</f>
         <v>32</v>
@@ -11120,8 +11050,8 @@
       <c r="C12" s="78" t="s">
         <v>381</v>
       </c>
-      <c r="D12" s="141"/>
-      <c r="E12" s="141"/>
+      <c r="D12" s="124"/>
+      <c r="E12" s="124"/>
       <c r="F12" s="79">
         <v>16</v>
       </c>
@@ -11183,8 +11113,8 @@
       <c r="C13" s="78" t="s">
         <v>382</v>
       </c>
-      <c r="D13" s="141"/>
-      <c r="E13" s="141"/>
+      <c r="D13" s="124"/>
+      <c r="E13" s="124"/>
       <c r="F13" s="79">
         <v>16</v>
       </c>
@@ -11338,28 +11268,12 @@
       <c r="T15" s="92"/>
     </row>
     <row r="16" spans="1:31">
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
+      <c r="F16" s="125"/>
+      <c r="G16" s="125"/>
+      <c r="H16" s="125"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="P9:S9"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
     <mergeCell ref="C3:S3"/>
     <mergeCell ref="Y3:AB3"/>
     <mergeCell ref="C5:E7"/>
@@ -11374,6 +11288,22 @@
     <mergeCell ref="N5:N6"/>
     <mergeCell ref="O5:O6"/>
     <mergeCell ref="P5:S5"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="P9:S9"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
   </mergeCells>
   <conditionalFormatting sqref="U11:X14">
     <cfRule type="iconSet" priority="2">
@@ -11410,9 +11340,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703084B0-7020-4228-BA63-87A3B98F18A3}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1"/>
@@ -20942,6 +20872,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001281E93D4CD8AF4592CEAE70F49402AE" ma:contentTypeVersion="19" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="bc27ca239ee5364de882bf49db749c36">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="07fe17d8-c930-4881-be9b-3b241872ecf2" xmlns:ns3="a516c34c-5f40-4b9f-bc5a-0e3bcef9c56f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dfd02d4500181950e6ebedca310b1d56" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -21199,15 +21138,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -21222,6 +21152,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{021E385F-31AC-44DC-AD80-9ADB528DC174}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0104D372-BA5B-4DD2-8ED7-FA9BFF6DAE56}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21237,14 +21175,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{021E385F-31AC-44DC-AD80-9ADB528DC174}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
cambio correo y avance
</commit_message>
<xml_diff>
--- a/data/FlujosTransaccionales.xlsx
+++ b/data/FlujosTransaccionales.xlsx
@@ -8,44 +8,44 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atcon\Desktop\Playwright\playwright-piloto2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A965DB8-9DFF-4759-8F74-A3DD026FB270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EAB182-F9D9-4DC6-A960-3051E3E2B8C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{522E3CD9-5E7D-4978-84C2-A91ECF51BF07}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Flujos" sheetId="19" r:id="rId1"/>
-    <sheet name="Flujos transaccionales " sheetId="18" r:id="rId2"/>
-    <sheet name="Matriz Modifica 745 24-09-2024" sheetId="16" state="hidden" r:id="rId3"/>
-    <sheet name="Matriz Modifica 750 25-09-2 " sheetId="17" state="hidden" r:id="rId4"/>
-    <sheet name="Matriz Modifica (737) 09-09-24" sheetId="15" state="hidden" r:id="rId5"/>
-    <sheet name="Matriz Modifica (715) 15-08-24" sheetId="14" state="hidden" r:id="rId6"/>
-    <sheet name="Matriz Modifica (707) 06-08-24" sheetId="13" state="hidden" r:id="rId7"/>
-    <sheet name="Matriz Modifica (702) 02-08-24" sheetId="12" state="hidden" r:id="rId8"/>
-    <sheet name="Matriz Modifica 25-07-2024" sheetId="11" state="hidden" r:id="rId9"/>
-    <sheet name="Matriz Modifica (696) 19-07-24" sheetId="8" state="hidden" r:id="rId10"/>
-    <sheet name="Matriz Modifica (683) 26 Jun 24" sheetId="7" state="hidden" r:id="rId11"/>
-    <sheet name="Matriz modificada  24 Junio 24" sheetId="6" state="hidden" r:id="rId12"/>
-    <sheet name="Matriz modificada  21 Junio 24" sheetId="4" state="hidden" r:id="rId13"/>
-    <sheet name="Matriz modificada" sheetId="2" state="hidden" r:id="rId14"/>
-    <sheet name="App" sheetId="9" r:id="rId15"/>
+    <sheet name="Hoja1" sheetId="20" r:id="rId2"/>
+    <sheet name="Flujos transaccionales " sheetId="18" r:id="rId3"/>
+    <sheet name="Matriz Modifica 745 24-09-2024" sheetId="16" state="hidden" r:id="rId4"/>
+    <sheet name="Matriz Modifica 750 25-09-2 " sheetId="17" state="hidden" r:id="rId5"/>
+    <sheet name="Matriz Modifica (737) 09-09-24" sheetId="15" state="hidden" r:id="rId6"/>
+    <sheet name="Matriz Modifica (715) 15-08-24" sheetId="14" state="hidden" r:id="rId7"/>
+    <sheet name="Matriz Modifica (707) 06-08-24" sheetId="13" state="hidden" r:id="rId8"/>
+    <sheet name="Matriz Modifica (702) 02-08-24" sheetId="12" state="hidden" r:id="rId9"/>
+    <sheet name="Matriz Modifica 25-07-2024" sheetId="11" state="hidden" r:id="rId10"/>
+    <sheet name="Matriz Modifica (696) 19-07-24" sheetId="8" state="hidden" r:id="rId11"/>
+    <sheet name="Matriz Modifica (683) 26 Jun 24" sheetId="7" state="hidden" r:id="rId12"/>
+    <sheet name="Matriz modificada  24 Junio 24" sheetId="6" state="hidden" r:id="rId13"/>
+    <sheet name="Matriz modificada  21 Junio 24" sheetId="4" state="hidden" r:id="rId14"/>
+    <sheet name="Matriz modificada" sheetId="2" state="hidden" r:id="rId15"/>
+    <sheet name="App" sheetId="9" r:id="rId16"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Flujos transaccionales '!$A$1:$J$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Matriz Modifica (683) 26 Jun 24'!$A$1:$M$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Matriz Modifica (696) 19-07-24'!$A$1:$M$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Matriz Modifica (702) 02-08-24'!$A$1:$M$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Matriz Modifica (707) 06-08-24'!$A$1:$M$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Matriz Modifica (715) 15-08-24'!$A$1:$M$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Matriz Modifica (737) 09-09-24'!$A$1:$M$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Matriz Modifica 25-07-2024'!$A$1:$M$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Matriz Modifica 745 24-09-2024'!$A$1:$M$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Matriz Modifica 750 25-09-2 '!$A$1:$M$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'Matriz modificada'!$A$1:$M$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Matriz modificada  21 Junio 24'!$A$1:$M$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Matriz modificada  24 Junio 24'!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Flujos transaccionales '!$A$1:$J$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Matriz Modifica (683) 26 Jun 24'!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Matriz Modifica (696) 19-07-24'!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Matriz Modifica (702) 02-08-24'!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Matriz Modifica (707) 06-08-24'!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Matriz Modifica (715) 15-08-24'!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Matriz Modifica (737) 09-09-24'!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Matriz Modifica 25-07-2024'!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Matriz Modifica 745 24-09-2024'!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Matriz Modifica 750 25-09-2 '!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'Matriz modificada'!$A$1:$M$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'Matriz modificada  21 Junio 24'!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Matriz modificada  24 Junio 24'!$A$1:$M$33</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3859" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3859" uniqueCount="405">
   <si>
     <t>ID</t>
   </si>
@@ -1501,6 +1501,18 @@
   </si>
   <si>
     <t>Pruebas Negativas</t>
+  </si>
+  <si>
+    <t>Vales</t>
+  </si>
+  <si>
+    <t>Tarjeta</t>
+  </si>
+  <si>
+    <t>Paypal</t>
+  </si>
+  <si>
+    <t>Entrega</t>
   </si>
 </sst>
 </file>
@@ -2127,7 +2139,7 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2553,6 +2565,7 @@
     <xf numFmtId="0" fontId="15" fillId="14" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -2935,10 +2948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7432F683-F664-4C95-88E4-2A9AFFFC0E8D}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2949,7 +2962,7 @@
     <col min="10" max="10" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" ht="11.4" customHeight="1">
       <c r="A1" t="s">
         <v>389</v>
       </c>
@@ -2983,67 +2996,21 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="B2" t="s">
-        <v>383</v>
+        <v>404</v>
       </c>
       <c r="C2" s="117"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="B3" t="s">
-        <v>384</v>
+        <v>401</v>
       </c>
       <c r="C3" s="117"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>385</v>
-      </c>
-      <c r="B4" t="s">
-        <v>385</v>
-      </c>
-      <c r="C4" s="117">
-        <v>4111111111111110</v>
-      </c>
-      <c r="I4" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>386</v>
-      </c>
-      <c r="B5" t="s">
-        <v>386</v>
-      </c>
-      <c r="C5" s="117">
-        <v>5105105105105100</v>
-      </c>
-      <c r="I5" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>387</v>
-      </c>
-      <c r="B6" t="s">
-        <v>387</v>
-      </c>
-      <c r="C6" s="117"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>388</v>
-      </c>
-      <c r="B7" t="s">
-        <v>388</v>
-      </c>
-      <c r="C7" s="117"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3051,6 +3018,1294 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181D2DB1-0637-49E2-BE78-B1DD33F2D937}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:N33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="3" width="9.109375" style="1"/>
+    <col min="4" max="4" width="37.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21" style="1" customWidth="1"/>
+    <col min="7" max="7" width="51.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="71.5546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="34.88671875" style="1" customWidth="1"/>
+    <col min="10" max="11" width="21" style="1" customWidth="1"/>
+    <col min="12" max="12" width="39.5546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="22.88671875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="21.44140625" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="11.44140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="28.8">
+      <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="144">
+      <c r="A2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2" s="19">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="M2" s="23" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="230.4" hidden="1">
+      <c r="A3" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" ht="230.4" hidden="1">
+      <c r="A4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="7">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" ht="244.8">
+      <c r="A5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="94" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="7">
+        <v>4</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="J5" s="93" t="s">
+        <v>80</v>
+      </c>
+      <c r="K5" s="95" t="s">
+        <v>242</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" ht="230.4" hidden="1">
+      <c r="A6" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="7">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" ht="201.6">
+      <c r="A7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C7" s="19">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="M7" s="23" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="316.8">
+      <c r="A8" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C8" s="19">
+        <v>7</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M8" s="23" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="316.8">
+      <c r="A9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C9" s="19">
+        <v>8</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M9" s="23" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="316.8">
+      <c r="A10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" s="19">
+        <v>9</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="K10" s="3"/>
+      <c r="L10" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M10" s="23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="316.8">
+      <c r="A11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C11" s="19">
+        <v>10</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="L11" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M11" s="23" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="374.4" hidden="1">
+      <c r="A12" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C12" s="19">
+        <v>11</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="J12" s="96" t="s">
+        <v>284</v>
+      </c>
+      <c r="K12" s="95"/>
+      <c r="L12" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M12" s="23" t="s">
+        <v>285</v>
+      </c>
+      <c r="N12" s="23" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="374.4" hidden="1">
+      <c r="A13" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C13" s="19">
+        <v>12</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="J13" s="96" t="s">
+        <v>284</v>
+      </c>
+      <c r="K13" s="3"/>
+      <c r="L13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M13" s="27" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="374.4" hidden="1">
+      <c r="A14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C14" s="19">
+        <v>13</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="J14" s="96" t="s">
+        <v>284</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M14" s="27" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="374.4" hidden="1">
+      <c r="A15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C15" s="19">
+        <v>14</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="J15" s="96" t="s">
+        <v>284</v>
+      </c>
+      <c r="K15" s="18"/>
+      <c r="L15" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M15" s="27" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="230.4" hidden="1">
+      <c r="C16" s="7">
+        <v>15</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="K16" s="3"/>
+      <c r="L16" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M16" s="3"/>
+    </row>
+    <row r="17" spans="1:14" ht="230.4" hidden="1">
+      <c r="C17" s="10">
+        <v>16</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="96" t="s">
+        <v>284</v>
+      </c>
+      <c r="K17" s="3"/>
+      <c r="L17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M17" s="3"/>
+    </row>
+    <row r="18" spans="1:14" ht="230.4" hidden="1">
+      <c r="A18" s="11"/>
+      <c r="C18" s="10">
+        <v>17</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="96" t="s">
+        <v>284</v>
+      </c>
+      <c r="K18" s="3"/>
+      <c r="L18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M18" s="3"/>
+    </row>
+    <row r="19" spans="1:14" ht="244.8">
+      <c r="A19" s="11"/>
+      <c r="B19" s="94" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" s="10">
+        <v>18</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J19" s="93" t="s">
+        <v>80</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="M19" s="3"/>
+    </row>
+    <row r="20" spans="1:14" ht="230.4" hidden="1">
+      <c r="C20" s="10">
+        <v>19</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="96" t="s">
+        <v>284</v>
+      </c>
+      <c r="K20" s="3"/>
+      <c r="L20" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M20" s="3"/>
+    </row>
+    <row r="21" spans="1:14" ht="201.6" hidden="1">
+      <c r="A21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C21" s="19">
+        <v>20</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="J21" s="96" t="s">
+        <v>284</v>
+      </c>
+      <c r="K21" s="24"/>
+      <c r="L21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="M21" s="27" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="201.6" hidden="1">
+      <c r="B22" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C22" s="19">
+        <v>21</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="J22" s="96" t="s">
+        <v>284</v>
+      </c>
+      <c r="K22" s="3"/>
+      <c r="L22" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="M22" s="27" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="316.8" hidden="1">
+      <c r="B23" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C23" s="19">
+        <v>22</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="J23" s="96" t="s">
+        <v>284</v>
+      </c>
+      <c r="K23" s="3"/>
+      <c r="L23" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M23" s="27" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="316.8" hidden="1">
+      <c r="A24" s="11"/>
+      <c r="B24" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C24" s="19">
+        <v>23</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="J24" s="96" t="s">
+        <v>284</v>
+      </c>
+      <c r="K24" s="3"/>
+      <c r="L24" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M24" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="316.8" hidden="1">
+      <c r="A25" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C25" s="19">
+        <v>24</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J25" s="96" t="s">
+        <v>284</v>
+      </c>
+      <c r="K25" s="18"/>
+      <c r="L25" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M25" s="27" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="316.8" hidden="1">
+      <c r="B26" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C26" s="19">
+        <v>25</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J26" s="96" t="s">
+        <v>284</v>
+      </c>
+      <c r="K26" s="3"/>
+      <c r="L26" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M26" s="27" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="374.4" hidden="1">
+      <c r="B27" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C27" s="19">
+        <v>26</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J27" s="96" t="s">
+        <v>284</v>
+      </c>
+      <c r="K27" s="3"/>
+      <c r="L27" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M27" s="27" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="374.4" hidden="1">
+      <c r="B28" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28" s="19">
+        <v>27</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J28" s="96" t="s">
+        <v>284</v>
+      </c>
+      <c r="K28" s="3"/>
+      <c r="L28" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M28" s="27" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="374.4" hidden="1">
+      <c r="A29" s="11"/>
+      <c r="B29" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29" s="19">
+        <v>28</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J29" s="96" t="s">
+        <v>284</v>
+      </c>
+      <c r="K29" s="3"/>
+      <c r="L29" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M29" s="27" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="374.4" hidden="1">
+      <c r="A30" s="11"/>
+      <c r="B30" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C30" s="19">
+        <v>29</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J30" s="96" t="s">
+        <v>284</v>
+      </c>
+      <c r="K30" s="3"/>
+      <c r="L30" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M30" s="27" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="230.4" hidden="1">
+      <c r="C31" s="12">
+        <v>30</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I31" s="3"/>
+      <c r="J31" s="96" t="s">
+        <v>284</v>
+      </c>
+      <c r="K31" s="3"/>
+      <c r="L31" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M31" s="3"/>
+    </row>
+    <row r="32" spans="1:14" ht="230.4" hidden="1">
+      <c r="A32" s="11"/>
+      <c r="B32" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C32" s="19">
+        <v>31</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J32" s="96" t="s">
+        <v>284</v>
+      </c>
+      <c r="K32" s="3"/>
+      <c r="L32" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="M32" s="27" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="230.4" hidden="1">
+      <c r="A33" s="11"/>
+      <c r="B33" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" s="19">
+        <v>32</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J33" s="96" t="s">
+        <v>284</v>
+      </c>
+      <c r="K33" s="3"/>
+      <c r="L33" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="M33" s="27" t="s">
+        <v>301</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:M33" xr:uid="{DCB37448-7794-4D71-83D8-79D0F3D93892}">
+    <filterColumn colId="9">
+      <filters>
+        <filter val="Exitoso"/>
+        <filter val="Fallado"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{E4A76D73-571B-4AE1-AFDD-5DEE4C349239}"/>
+    <hyperlink ref="L3:L5" r:id="rId2" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{0AB495DA-B9FA-45DC-87C3-28FFA1070330}"/>
+    <hyperlink ref="L6" r:id="rId3" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{0ADBCDDB-FA7D-452D-B810-65CC7CD488E6}"/>
+    <hyperlink ref="L7:L12" r:id="rId4" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{293E7FA0-1486-4A9C-8C12-675476076B32}"/>
+    <hyperlink ref="L16" r:id="rId5" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{CF97AA96-CE0E-45A0-A793-6B077114AAD9}"/>
+    <hyperlink ref="L8" r:id="rId6" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{5CA41B4B-0C87-4544-9109-39D3C65313DC}"/>
+    <hyperlink ref="L9" r:id="rId7" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{498AF637-15BF-4ECE-B7D4-76D2C03F4299}"/>
+    <hyperlink ref="L10" r:id="rId8" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{2BAEB929-E89C-417D-8F77-2FD19B348432}"/>
+    <hyperlink ref="L11" r:id="rId9" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{74E8F51E-B446-49EB-9539-3459C0CC0642}"/>
+    <hyperlink ref="L13" r:id="rId10" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{52DB0A38-97D0-44EF-9F78-CC13534B6585}"/>
+    <hyperlink ref="L14" r:id="rId11" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{77CFF23E-9C46-42B9-97DD-CA3EF140CAA3}"/>
+    <hyperlink ref="L15" r:id="rId12" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{5EDE640B-9D4D-41A7-882C-F98C3E37ECC9}"/>
+    <hyperlink ref="L17:L19" r:id="rId13" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{10656951-D0AF-4326-A241-6E4045B6A1F1}"/>
+    <hyperlink ref="L20" r:id="rId14" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{E37B5A9D-FD89-4AB5-AE0F-833BD6C162D9}"/>
+    <hyperlink ref="L21:L27" r:id="rId15" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{AE4D2126-5010-4967-8BBA-96BA229210FA}"/>
+    <hyperlink ref="L31" r:id="rId16" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{5DD26D7C-D651-4A38-BDA6-05B9D505ED07}"/>
+    <hyperlink ref="L23" r:id="rId17" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{1301856F-F9DD-4B4D-84E7-770D844471FE}"/>
+    <hyperlink ref="L24" r:id="rId18" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{51681362-69EA-4E52-B9D3-C0BEBB0C7D14}"/>
+    <hyperlink ref="L25" r:id="rId19" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{9198CE4C-F804-44EB-8F72-C2EFFCCEDB6E}"/>
+    <hyperlink ref="L26" r:id="rId20" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{7E3B2F0B-CC64-4C1C-B91B-E04272F396FA}"/>
+    <hyperlink ref="L28" r:id="rId21" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{1F55B09A-4230-49BF-9916-6ECC3F21CCEB}"/>
+    <hyperlink ref="L29" r:id="rId22" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{3F45471A-B863-4BC3-8E5A-1AF465192FAC}"/>
+    <hyperlink ref="L30" r:id="rId23" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{F5223605-24A9-497D-B5D2-D3A7EF1C9390}"/>
+    <hyperlink ref="L32" r:id="rId24" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{6399BCC3-EBCE-47DE-A2D1-1177A7DE56AD}"/>
+    <hyperlink ref="L33" r:id="rId25" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{BCE13C7B-9926-489A-8738-F5CEA63D81D8}"/>
+    <hyperlink ref="N12" r:id="rId26" xr:uid="{6E1FE270-6990-49D5-9DFD-A8F262E69B68}"/>
+    <hyperlink ref="M2" r:id="rId27" xr:uid="{9BF67833-FAD1-45A5-AA94-B09EFA35F7E9}"/>
+    <hyperlink ref="M7" r:id="rId28" xr:uid="{2ADB50C7-2C7D-420F-84FF-8D729E37B3D6}"/>
+    <hyperlink ref="M13" r:id="rId29" xr:uid="{D7371BED-E067-49E7-959A-C3DC1BE40BAD}"/>
+    <hyperlink ref="M8" r:id="rId30" xr:uid="{0046F648-3672-41E5-820D-078EA653F299}"/>
+    <hyperlink ref="M14" r:id="rId31" xr:uid="{F53696A7-51B1-45F9-A40C-FCAED0C38413}"/>
+    <hyperlink ref="M15" r:id="rId32" xr:uid="{2455ED56-D868-4273-AB5B-29305818EF98}"/>
+    <hyperlink ref="M25" r:id="rId33" xr:uid="{5979A387-AD13-493E-95D5-158BCD2AF302}"/>
+    <hyperlink ref="M26" r:id="rId34" xr:uid="{90875164-F117-4FB8-BD2E-BEF35D4E699D}"/>
+    <hyperlink ref="M27" r:id="rId35" xr:uid="{2803C341-27C6-45A6-9E6A-0B4E9791B04E}"/>
+    <hyperlink ref="M28" r:id="rId36" xr:uid="{DBAD2E0A-5C64-44A6-A7F0-385A9D3AA955}"/>
+    <hyperlink ref="M29" r:id="rId37" xr:uid="{8E173185-C38A-43BB-BFA7-DA12DF70B28D}"/>
+    <hyperlink ref="M30" r:id="rId38" xr:uid="{86661650-5EF8-4A8D-931A-FD7C71A2FA79}"/>
+    <hyperlink ref="M32" r:id="rId39" xr:uid="{08CDBF07-19F6-457F-8D36-EDB6A7C462AD}"/>
+    <hyperlink ref="M33" r:id="rId40" xr:uid="{720F1E59-A76D-4B3A-89EA-03CF35EEF331}"/>
+    <hyperlink ref="M9" r:id="rId41" xr:uid="{D041E33F-7657-40BA-95B6-18F99D5ECA2C}"/>
+    <hyperlink ref="M21" r:id="rId42" xr:uid="{7A256CA2-32B1-4BF5-AD3E-0D88B3570319}"/>
+    <hyperlink ref="M10" r:id="rId43" xr:uid="{235DC055-8A69-47C7-B5F0-21D4048573F3}"/>
+    <hyperlink ref="M23" r:id="rId44" xr:uid="{1B2CA557-E42A-417A-BDEF-66941F8FD4E8}"/>
+    <hyperlink ref="M22" r:id="rId45" xr:uid="{4B4589C0-A721-47AB-8D5D-4E7C8836BC93}"/>
+    <hyperlink ref="M11" r:id="rId46" xr:uid="{B1FD90A6-4BC0-41E9-9006-204E3AFD8966}"/>
+    <hyperlink ref="M24" r:id="rId47" xr:uid="{08F162FC-F970-4F6E-A4FB-5B9511385C47}"/>
+    <hyperlink ref="M12" r:id="rId48" xr:uid="{8F7CC884-16B2-4065-9E0A-4D6FB500D560}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F1E6B3-AE0E-4F82-8CE5-818E954EB8E9}">
   <dimension ref="A1:N33"/>
   <sheetViews>
@@ -4314,7 +5569,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC121400-37A7-45CB-AB75-E80E51530A57}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M33"/>
@@ -5488,7 +6743,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6B80E1-D096-4AA5-AD9A-02A7B8F61FD8}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M33"/>
@@ -6676,7 +7931,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D869C7AD-B81B-46EF-9D92-1D8A4BF4B6FB}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M33"/>
@@ -7825,7 +9080,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB37448-7794-4D71-83D8-79D0F3D93892}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M33"/>
@@ -8968,7 +10223,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF491AA-1038-4BD9-85C2-55A46D475EEA}">
   <dimension ref="A1:AE16"/>
   <sheetViews>
@@ -11337,12 +12592,102 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC98DD0-04DF-46E2-AE89-603FE9DF8BD7}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="17.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="116" t="s">
+        <v>383</v>
+      </c>
+      <c r="B1" s="116" t="s">
+        <v>402</v>
+      </c>
+      <c r="C1" s="145"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="116"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="116" t="s">
+        <v>384</v>
+      </c>
+      <c r="B2" s="116" t="s">
+        <v>402</v>
+      </c>
+      <c r="C2" s="145"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="116" t="s">
+        <v>385</v>
+      </c>
+      <c r="B3" s="116" t="s">
+        <v>402</v>
+      </c>
+      <c r="C3" s="145">
+        <v>4111111111111110</v>
+      </c>
+      <c r="D3" s="116"/>
+      <c r="E3" s="116"/>
+      <c r="F3" s="116"/>
+      <c r="G3" s="116"/>
+      <c r="H3" s="116"/>
+      <c r="I3" s="116" t="s">
+        <v>398</v>
+      </c>
+      <c r="J3" s="116"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="116" t="s">
+        <v>386</v>
+      </c>
+      <c r="B4" s="116" t="s">
+        <v>403</v>
+      </c>
+      <c r="C4" s="145">
+        <v>5105105105105100</v>
+      </c>
+      <c r="D4" s="116"/>
+      <c r="E4" s="116"/>
+      <c r="F4" s="116"/>
+      <c r="G4" s="116"/>
+      <c r="H4" s="116"/>
+      <c r="I4" s="116" t="s">
+        <v>399</v>
+      </c>
+      <c r="J4" s="116"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703084B0-7020-4228-BA63-87A3B98F18A3}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1"/>
@@ -11865,7 +13210,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{276724DB-1A94-4063-A318-86352BC79020}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N33"/>
@@ -13198,7 +14543,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FB9472-2E2F-4C8E-8379-6B5FA0E476A2}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N33"/>
@@ -14493,7 +15838,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDB9C14-3C91-42A1-B5CD-64E20BDBD4B5}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N33"/>
@@ -15726,7 +17071,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31CE0FA-6A3C-4645-AE25-E75B2D5D9895}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N33"/>
@@ -16940,7 +18285,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F87DEE-8A67-4F56-AB92-709EFA44E565}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N33"/>
@@ -18252,7 +19597,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE180F16-E1DA-4BB3-8569-5BCDA49E36FB}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N33"/>
@@ -19578,1294 +20923,6 @@
     <hyperlink ref="M28" r:id="rId46" xr:uid="{B8785A92-9B80-444E-B239-EDA194ACFCC3}"/>
     <hyperlink ref="M32" r:id="rId47" xr:uid="{ECAC17AD-1E1A-4E06-AAD8-99620C4252C7}"/>
     <hyperlink ref="M33" r:id="rId48" xr:uid="{DE3B80FD-E607-4134-841E-8005649988FB}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181D2DB1-0637-49E2-BE78-B1DD33F2D937}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:N33"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2" max="3" width="9.109375" style="1"/>
-    <col min="4" max="4" width="37.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="40" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21" style="1" customWidth="1"/>
-    <col min="7" max="7" width="51.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="71.5546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="34.88671875" style="1" customWidth="1"/>
-    <col min="10" max="11" width="21" style="1" customWidth="1"/>
-    <col min="12" max="12" width="39.5546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="22.88671875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="21.44140625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.44140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="28.8">
-      <c r="B1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="N1" s="30" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="144">
-      <c r="A2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C2" s="19">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="M2" s="23" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="230.4" hidden="1">
-      <c r="A3" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="7">
-        <v>2</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:14" ht="230.4" hidden="1">
-      <c r="A4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="7">
-        <v>3</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="M4" s="3"/>
-    </row>
-    <row r="5" spans="1:14" ht="244.8">
-      <c r="A5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="94" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="7">
-        <v>4</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="J5" s="93" t="s">
-        <v>80</v>
-      </c>
-      <c r="K5" s="95" t="s">
-        <v>242</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="M5" s="3"/>
-    </row>
-    <row r="6" spans="1:14" ht="230.4" hidden="1">
-      <c r="A6" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="7">
-        <v>5</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="M6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" ht="201.6">
-      <c r="A7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C7" s="19">
-        <v>6</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>273</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="K7" s="3"/>
-      <c r="L7" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="M7" s="23" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="316.8">
-      <c r="A8" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C8" s="19">
-        <v>7</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M8" s="23" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="316.8">
-      <c r="A9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C9" s="19">
-        <v>8</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M9" s="23" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="316.8">
-      <c r="A10" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C10" s="19">
-        <v>9</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M10" s="23" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="316.8">
-      <c r="A11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C11" s="19">
-        <v>10</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="K11" s="3"/>
-      <c r="L11" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M11" s="23" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="374.4" hidden="1">
-      <c r="A12" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C12" s="19">
-        <v>11</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="J12" s="96" t="s">
-        <v>284</v>
-      </c>
-      <c r="K12" s="95"/>
-      <c r="L12" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M12" s="23" t="s">
-        <v>285</v>
-      </c>
-      <c r="N12" s="23" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="374.4" hidden="1">
-      <c r="A13" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C13" s="19">
-        <v>12</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="J13" s="96" t="s">
-        <v>284</v>
-      </c>
-      <c r="K13" s="3"/>
-      <c r="L13" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M13" s="27" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="374.4" hidden="1">
-      <c r="A14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C14" s="19">
-        <v>13</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="J14" s="96" t="s">
-        <v>284</v>
-      </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M14" s="27" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="374.4" hidden="1">
-      <c r="A15" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C15" s="19">
-        <v>14</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="J15" s="96" t="s">
-        <v>284</v>
-      </c>
-      <c r="K15" s="18"/>
-      <c r="L15" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M15" s="27" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="230.4" hidden="1">
-      <c r="C16" s="7">
-        <v>15</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="K16" s="3"/>
-      <c r="L16" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="M16" s="3"/>
-    </row>
-    <row r="17" spans="1:14" ht="230.4" hidden="1">
-      <c r="C17" s="10">
-        <v>16</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="96" t="s">
-        <v>284</v>
-      </c>
-      <c r="K17" s="3"/>
-      <c r="L17" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="M17" s="3"/>
-    </row>
-    <row r="18" spans="1:14" ht="230.4" hidden="1">
-      <c r="A18" s="11"/>
-      <c r="C18" s="10">
-        <v>17</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="96" t="s">
-        <v>284</v>
-      </c>
-      <c r="K18" s="3"/>
-      <c r="L18" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="M18" s="3"/>
-    </row>
-    <row r="19" spans="1:14" ht="244.8">
-      <c r="A19" s="11"/>
-      <c r="B19" s="94" t="s">
-        <v>116</v>
-      </c>
-      <c r="C19" s="10">
-        <v>18</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="J19" s="93" t="s">
-        <v>80</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="M19" s="3"/>
-    </row>
-    <row r="20" spans="1:14" ht="230.4" hidden="1">
-      <c r="C20" s="10">
-        <v>19</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="96" t="s">
-        <v>284</v>
-      </c>
-      <c r="K20" s="3"/>
-      <c r="L20" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="M20" s="3"/>
-    </row>
-    <row r="21" spans="1:14" ht="201.6" hidden="1">
-      <c r="A21" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C21" s="19">
-        <v>20</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="J21" s="96" t="s">
-        <v>284</v>
-      </c>
-      <c r="K21" s="24"/>
-      <c r="L21" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="M21" s="27" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="201.6" hidden="1">
-      <c r="B22" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C22" s="19">
-        <v>21</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="J22" s="96" t="s">
-        <v>284</v>
-      </c>
-      <c r="K22" s="3"/>
-      <c r="L22" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="M22" s="27" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="316.8" hidden="1">
-      <c r="B23" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C23" s="19">
-        <v>22</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="J23" s="96" t="s">
-        <v>284</v>
-      </c>
-      <c r="K23" s="3"/>
-      <c r="L23" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M23" s="27" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="316.8" hidden="1">
-      <c r="A24" s="11"/>
-      <c r="B24" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C24" s="19">
-        <v>23</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>293</v>
-      </c>
-      <c r="J24" s="96" t="s">
-        <v>284</v>
-      </c>
-      <c r="K24" s="3"/>
-      <c r="L24" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M24" s="27" t="s">
-        <v>257</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="316.8" hidden="1">
-      <c r="A25" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C25" s="19">
-        <v>24</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="J25" s="96" t="s">
-        <v>284</v>
-      </c>
-      <c r="K25" s="18"/>
-      <c r="L25" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M25" s="27" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="316.8" hidden="1">
-      <c r="B26" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C26" s="19">
-        <v>25</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="J26" s="96" t="s">
-        <v>284</v>
-      </c>
-      <c r="K26" s="3"/>
-      <c r="L26" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M26" s="27" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="374.4" hidden="1">
-      <c r="B27" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C27" s="19">
-        <v>26</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="J27" s="96" t="s">
-        <v>284</v>
-      </c>
-      <c r="K27" s="3"/>
-      <c r="L27" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M27" s="27" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="374.4" hidden="1">
-      <c r="B28" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C28" s="19">
-        <v>27</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="J28" s="96" t="s">
-        <v>284</v>
-      </c>
-      <c r="K28" s="3"/>
-      <c r="L28" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M28" s="27" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="374.4" hidden="1">
-      <c r="A29" s="11"/>
-      <c r="B29" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C29" s="19">
-        <v>28</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="J29" s="96" t="s">
-        <v>284</v>
-      </c>
-      <c r="K29" s="3"/>
-      <c r="L29" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M29" s="27" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="374.4" hidden="1">
-      <c r="A30" s="11"/>
-      <c r="B30" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C30" s="19">
-        <v>29</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="J30" s="96" t="s">
-        <v>284</v>
-      </c>
-      <c r="K30" s="3"/>
-      <c r="L30" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M30" s="27" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" ht="230.4" hidden="1">
-      <c r="C31" s="12">
-        <v>30</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I31" s="3"/>
-      <c r="J31" s="96" t="s">
-        <v>284</v>
-      </c>
-      <c r="K31" s="3"/>
-      <c r="L31" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="M31" s="3"/>
-    </row>
-    <row r="32" spans="1:14" ht="230.4" hidden="1">
-      <c r="A32" s="11"/>
-      <c r="B32" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C32" s="19">
-        <v>31</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="J32" s="96" t="s">
-        <v>284</v>
-      </c>
-      <c r="K32" s="3"/>
-      <c r="L32" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="M32" s="27" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="230.4" hidden="1">
-      <c r="A33" s="11"/>
-      <c r="B33" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C33" s="19">
-        <v>32</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="J33" s="96" t="s">
-        <v>284</v>
-      </c>
-      <c r="K33" s="3"/>
-      <c r="L33" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="M33" s="27" t="s">
-        <v>301</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:M33" xr:uid="{DCB37448-7794-4D71-83D8-79D0F3D93892}">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="Exitoso"/>
-        <filter val="Fallado"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{E4A76D73-571B-4AE1-AFDD-5DEE4C349239}"/>
-    <hyperlink ref="L3:L5" r:id="rId2" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{0AB495DA-B9FA-45DC-87C3-28FFA1070330}"/>
-    <hyperlink ref="L6" r:id="rId3" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{0ADBCDDB-FA7D-452D-B810-65CC7CD488E6}"/>
-    <hyperlink ref="L7:L12" r:id="rId4" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{293E7FA0-1486-4A9C-8C12-675476076B32}"/>
-    <hyperlink ref="L16" r:id="rId5" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{CF97AA96-CE0E-45A0-A793-6B077114AAD9}"/>
-    <hyperlink ref="L8" r:id="rId6" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{5CA41B4B-0C87-4544-9109-39D3C65313DC}"/>
-    <hyperlink ref="L9" r:id="rId7" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{498AF637-15BF-4ECE-B7D4-76D2C03F4299}"/>
-    <hyperlink ref="L10" r:id="rId8" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{2BAEB929-E89C-417D-8F77-2FD19B348432}"/>
-    <hyperlink ref="L11" r:id="rId9" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{74E8F51E-B446-49EB-9539-3459C0CC0642}"/>
-    <hyperlink ref="L13" r:id="rId10" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{52DB0A38-97D0-44EF-9F78-CC13534B6585}"/>
-    <hyperlink ref="L14" r:id="rId11" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{77CFF23E-9C46-42B9-97DD-CA3EF140CAA3}"/>
-    <hyperlink ref="L15" r:id="rId12" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{5EDE640B-9D4D-41A7-882C-F98C3E37ECC9}"/>
-    <hyperlink ref="L17:L19" r:id="rId13" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{10656951-D0AF-4326-A241-6E4045B6A1F1}"/>
-    <hyperlink ref="L20" r:id="rId14" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{E37B5A9D-FD89-4AB5-AE0F-833BD6C162D9}"/>
-    <hyperlink ref="L21:L27" r:id="rId15" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{AE4D2126-5010-4967-8BBA-96BA229210FA}"/>
-    <hyperlink ref="L31" r:id="rId16" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{5DD26D7C-D651-4A38-BDA6-05B9D505ED07}"/>
-    <hyperlink ref="L23" r:id="rId17" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{1301856F-F9DD-4B4D-84E7-770D844471FE}"/>
-    <hyperlink ref="L24" r:id="rId18" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{51681362-69EA-4E52-B9D3-C0BEBB0C7D14}"/>
-    <hyperlink ref="L25" r:id="rId19" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{9198CE4C-F804-44EB-8F72-C2EFFCCEDB6E}"/>
-    <hyperlink ref="L26" r:id="rId20" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{7E3B2F0B-CC64-4C1C-B91B-E04272F396FA}"/>
-    <hyperlink ref="L28" r:id="rId21" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{1F55B09A-4230-49BF-9916-6ECC3F21CCEB}"/>
-    <hyperlink ref="L29" r:id="rId22" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{3F45471A-B863-4BC3-8E5A-1AF465192FAC}"/>
-    <hyperlink ref="L30" r:id="rId23" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{F5223605-24A9-497D-B5D2-D3A7EF1C9390}"/>
-    <hyperlink ref="L32" r:id="rId24" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{6399BCC3-EBCE-47DE-A2D1-1177A7DE56AD}"/>
-    <hyperlink ref="L33" r:id="rId25" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{BCE13C7B-9926-489A-8738-F5CEA63D81D8}"/>
-    <hyperlink ref="N12" r:id="rId26" xr:uid="{6E1FE270-6990-49D5-9DFD-A8F262E69B68}"/>
-    <hyperlink ref="M2" r:id="rId27" xr:uid="{9BF67833-FAD1-45A5-AA94-B09EFA35F7E9}"/>
-    <hyperlink ref="M7" r:id="rId28" xr:uid="{2ADB50C7-2C7D-420F-84FF-8D729E37B3D6}"/>
-    <hyperlink ref="M13" r:id="rId29" xr:uid="{D7371BED-E067-49E7-959A-C3DC1BE40BAD}"/>
-    <hyperlink ref="M8" r:id="rId30" xr:uid="{0046F648-3672-41E5-820D-078EA653F299}"/>
-    <hyperlink ref="M14" r:id="rId31" xr:uid="{F53696A7-51B1-45F9-A40C-FCAED0C38413}"/>
-    <hyperlink ref="M15" r:id="rId32" xr:uid="{2455ED56-D868-4273-AB5B-29305818EF98}"/>
-    <hyperlink ref="M25" r:id="rId33" xr:uid="{5979A387-AD13-493E-95D5-158BCD2AF302}"/>
-    <hyperlink ref="M26" r:id="rId34" xr:uid="{90875164-F117-4FB8-BD2E-BEF35D4E699D}"/>
-    <hyperlink ref="M27" r:id="rId35" xr:uid="{2803C341-27C6-45A6-9E6A-0B4E9791B04E}"/>
-    <hyperlink ref="M28" r:id="rId36" xr:uid="{DBAD2E0A-5C64-44A6-A7F0-385A9D3AA955}"/>
-    <hyperlink ref="M29" r:id="rId37" xr:uid="{8E173185-C38A-43BB-BFA7-DA12DF70B28D}"/>
-    <hyperlink ref="M30" r:id="rId38" xr:uid="{86661650-5EF8-4A8D-931A-FD7C71A2FA79}"/>
-    <hyperlink ref="M32" r:id="rId39" xr:uid="{08CDBF07-19F6-457F-8D36-EDB6A7C462AD}"/>
-    <hyperlink ref="M33" r:id="rId40" xr:uid="{720F1E59-A76D-4B3A-89EA-03CF35EEF331}"/>
-    <hyperlink ref="M9" r:id="rId41" xr:uid="{D041E33F-7657-40BA-95B6-18F99D5ECA2C}"/>
-    <hyperlink ref="M21" r:id="rId42" xr:uid="{7A256CA2-32B1-4BF5-AD3E-0D88B3570319}"/>
-    <hyperlink ref="M10" r:id="rId43" xr:uid="{235DC055-8A69-47C7-B5F0-21D4048573F3}"/>
-    <hyperlink ref="M23" r:id="rId44" xr:uid="{1B2CA557-E42A-417A-BDEF-66941F8FD4E8}"/>
-    <hyperlink ref="M22" r:id="rId45" xr:uid="{4B4589C0-A721-47AB-8D5D-4E7C8836BC93}"/>
-    <hyperlink ref="M11" r:id="rId46" xr:uid="{B1FD90A6-4BC0-41E9-9006-204E3AFD8966}"/>
-    <hyperlink ref="M24" r:id="rId47" xr:uid="{08F162FC-F970-4F6E-A4FB-5B9511385C47}"/>
-    <hyperlink ref="M12" r:id="rId48" xr:uid="{8F7CC884-16B2-4065-9E0A-4D6FB500D560}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cambios en flujos transaccionales
</commit_message>
<xml_diff>
--- a/data/FlujosTransaccionales.xlsx
+++ b/data/FlujosTransaccionales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atcon\Desktop\Playwright\playwright-piloto2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EAB182-F9D9-4DC6-A960-3051E3E2B8C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D6C1A9-A3D2-449B-B61C-DA7F53C21F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{522E3CD9-5E7D-4978-84C2-A91ECF51BF07}"/>
   </bookViews>
@@ -2951,7 +2951,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
se agrega nuevo correo
</commit_message>
<xml_diff>
--- a/data/FlujosTransaccionales.xlsx
+++ b/data/FlujosTransaccionales.xlsx
@@ -8,44 +8,46 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atcon\Desktop\Playwright\playwright-piloto2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D6C1A9-A3D2-449B-B61C-DA7F53C21F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9AC664-5EFC-4B41-9A7C-EEBC5ADFC523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{522E3CD9-5E7D-4978-84C2-A91ECF51BF07}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{522E3CD9-5E7D-4978-84C2-A91ECF51BF07}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Flujos" sheetId="19" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="20" r:id="rId2"/>
-    <sheet name="Flujos transaccionales " sheetId="18" r:id="rId3"/>
-    <sheet name="Matriz Modifica 745 24-09-2024" sheetId="16" state="hidden" r:id="rId4"/>
-    <sheet name="Matriz Modifica 750 25-09-2 " sheetId="17" state="hidden" r:id="rId5"/>
-    <sheet name="Matriz Modifica (737) 09-09-24" sheetId="15" state="hidden" r:id="rId6"/>
-    <sheet name="Matriz Modifica (715) 15-08-24" sheetId="14" state="hidden" r:id="rId7"/>
-    <sheet name="Matriz Modifica (707) 06-08-24" sheetId="13" state="hidden" r:id="rId8"/>
-    <sheet name="Matriz Modifica (702) 02-08-24" sheetId="12" state="hidden" r:id="rId9"/>
-    <sheet name="Matriz Modifica 25-07-2024" sheetId="11" state="hidden" r:id="rId10"/>
-    <sheet name="Matriz Modifica (696) 19-07-24" sheetId="8" state="hidden" r:id="rId11"/>
-    <sheet name="Matriz Modifica (683) 26 Jun 24" sheetId="7" state="hidden" r:id="rId12"/>
-    <sheet name="Matriz modificada  24 Junio 24" sheetId="6" state="hidden" r:id="rId13"/>
-    <sheet name="Matriz modificada  21 Junio 24" sheetId="4" state="hidden" r:id="rId14"/>
-    <sheet name="Matriz modificada" sheetId="2" state="hidden" r:id="rId15"/>
-    <sheet name="App" sheetId="9" r:id="rId16"/>
+    <sheet name="Validaciones Tarjeta" sheetId="20" r:id="rId2"/>
+    <sheet name="FlujosPruebas" sheetId="21" r:id="rId3"/>
+    <sheet name="Flujos transaccionales " sheetId="18" r:id="rId4"/>
+    <sheet name="Matriz Modifica 745 24-09-2024" sheetId="16" state="hidden" r:id="rId5"/>
+    <sheet name="Matriz Modifica 750 25-09-2 " sheetId="17" state="hidden" r:id="rId6"/>
+    <sheet name="Matriz Modifica (737) 09-09-24" sheetId="15" state="hidden" r:id="rId7"/>
+    <sheet name="Matriz Modifica (715) 15-08-24" sheetId="14" state="hidden" r:id="rId8"/>
+    <sheet name="Matriz Modifica (707) 06-08-24" sheetId="13" state="hidden" r:id="rId9"/>
+    <sheet name="Matriz Modifica (702) 02-08-24" sheetId="12" state="hidden" r:id="rId10"/>
+    <sheet name="Matriz Modifica 25-07-2024" sheetId="11" state="hidden" r:id="rId11"/>
+    <sheet name="Matriz Modifica (696) 19-07-24" sheetId="8" state="hidden" r:id="rId12"/>
+    <sheet name="Matriz Modifica (683) 26 Jun 24" sheetId="7" state="hidden" r:id="rId13"/>
+    <sheet name="Matriz modificada  24 Junio 24" sheetId="6" state="hidden" r:id="rId14"/>
+    <sheet name="Matriz modificada  21 Junio 24" sheetId="4" state="hidden" r:id="rId15"/>
+    <sheet name="Matriz modificada" sheetId="2" state="hidden" r:id="rId16"/>
+    <sheet name="App" sheetId="9" r:id="rId17"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Flujos transaccionales '!$A$1:$J$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Matriz Modifica (683) 26 Jun 24'!$A$1:$M$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Matriz Modifica (696) 19-07-24'!$A$1:$M$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Matriz Modifica (702) 02-08-24'!$A$1:$M$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Matriz Modifica (707) 06-08-24'!$A$1:$M$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Matriz Modifica (715) 15-08-24'!$A$1:$M$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Matriz Modifica (737) 09-09-24'!$A$1:$M$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Matriz Modifica 25-07-2024'!$A$1:$M$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Matriz Modifica 745 24-09-2024'!$A$1:$M$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Matriz Modifica 750 25-09-2 '!$A$1:$M$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'Matriz modificada'!$A$1:$M$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'Matriz modificada  21 Junio 24'!$A$1:$M$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Matriz modificada  24 Junio 24'!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Flujos transaccionales '!$A$1:$J$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Matriz Modifica (683) 26 Jun 24'!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Matriz Modifica (696) 19-07-24'!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Matriz Modifica (702) 02-08-24'!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Matriz Modifica (707) 06-08-24'!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Matriz Modifica (715) 15-08-24'!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Matriz Modifica (737) 09-09-24'!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Matriz Modifica 25-07-2024'!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Matriz Modifica 745 24-09-2024'!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Matriz Modifica 750 25-09-2 '!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">'Matriz modificada'!$A$1:$M$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'Matriz modificada  21 Junio 24'!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'Matriz modificada  24 Junio 24'!$A$1:$M$33</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -66,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3859" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4022" uniqueCount="453">
   <si>
     <t>ID</t>
   </si>
@@ -1494,15 +1496,6 @@
     <t>Tipo</t>
   </si>
   <si>
-    <t>Debito</t>
-  </si>
-  <si>
-    <t>Credito</t>
-  </si>
-  <si>
-    <t>Pruebas Negativas</t>
-  </si>
-  <si>
     <t>Vales</t>
   </si>
   <si>
@@ -1513,13 +1506,166 @@
   </si>
   <si>
     <t>Entrega</t>
+  </si>
+  <si>
+    <t>4111111111111111</t>
+  </si>
+  <si>
+    <t>4222222222222220</t>
+  </si>
+  <si>
+    <t>4000000000000069</t>
+  </si>
+  <si>
+    <t>Expirada</t>
+  </si>
+  <si>
+    <t>Rechazada</t>
+  </si>
+  <si>
+    <t>Fondos Insuficientes</t>
+  </si>
+  <si>
+    <t>370000000000002</t>
+  </si>
+  <si>
+    <t>Banco</t>
+  </si>
+  <si>
+    <t>BANAMEX</t>
+  </si>
+  <si>
+    <t>AMERICAN EXPRESS</t>
+  </si>
+  <si>
+    <t>345678000000007</t>
+  </si>
+  <si>
+    <t>Débito</t>
+  </si>
+  <si>
+    <t>Crédito</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Escenario</t>
+  </si>
+  <si>
+    <t>AnoExpirado</t>
+  </si>
+  <si>
+    <t>MesExpirado</t>
+  </si>
+  <si>
+    <t>Carnet</t>
+  </si>
+  <si>
+    <t>5062541600005232</t>
+  </si>
+  <si>
+    <t>5064050100000063</t>
+  </si>
+  <si>
+    <t>5064510000300020</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>Nuevo</t>
+  </si>
+  <si>
+    <t>Recurrente</t>
+  </si>
+  <si>
+    <t>Pago con tarjeta de crédito / débito (Super + Vinos y licores)</t>
+  </si>
+  <si>
+    <t>realiza una segunda compra</t>
+  </si>
+  <si>
+    <t>Repetir compra</t>
+  </si>
+  <si>
+    <t>Pago con Vales de colaborador chedraui (Super)</t>
+  </si>
+  <si>
+    <t>Pago contra Entrega (DHL)</t>
+  </si>
+  <si>
+    <t>Pago contra Entrega (Super)</t>
+  </si>
+  <si>
+    <t>Pago con PAYPAL (Super)</t>
+  </si>
+  <si>
+    <t>Pago Con puntos BBVA (Super)</t>
+  </si>
+  <si>
+    <t>Pago con Vales de despensa (Super)</t>
+  </si>
+  <si>
+    <t>Pago con tarjeta de crédito / débito (Flete)</t>
+  </si>
+  <si>
+    <t>Pago con tarjeta de crédito / débito (DHL)</t>
+  </si>
+  <si>
+    <t>Joaquin Roberto Soto Castillo</t>
+  </si>
+  <si>
+    <t>Activos</t>
+  </si>
+  <si>
+    <t>Sucursal</t>
+  </si>
+  <si>
+    <t>Super</t>
+  </si>
+  <si>
+    <t>Flete</t>
+  </si>
+  <si>
+    <t>DHL</t>
+  </si>
+  <si>
+    <t>Refrigerador</t>
+  </si>
+  <si>
+    <t>Consola</t>
+  </si>
+  <si>
+    <t>Aguacate, Cebolla, Platano</t>
+  </si>
+  <si>
+    <t>Enviadero</t>
+  </si>
+  <si>
+    <t>Flete, Enviadero, Super</t>
+  </si>
+  <si>
+    <t>Aguacate, Cebolla, Platano, Refrigerador, Consola</t>
+  </si>
+  <si>
+    <t>TipoTienda</t>
+  </si>
+  <si>
+    <t>Interlomas</t>
+  </si>
+  <si>
+    <t>Santa fe</t>
+  </si>
+  <si>
+    <t>Polanco</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1690,6 +1836,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF272626"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="19">
@@ -2139,7 +2291,7 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2484,54 +2636,6 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="13" fillId="14" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="13" fillId="14" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2565,7 +2669,57 @@
     <xf numFmtId="0" fontId="15" fillId="14" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="13" fillId="14" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="13" fillId="14" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -2948,10 +3102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7432F683-F664-4C95-88E4-2A9AFFFC0E8D}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2962,7 +3116,7 @@
     <col min="10" max="10" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="11.4" customHeight="1">
+    <row r="1" spans="1:3" ht="11.4" customHeight="1">
       <c r="A1" t="s">
         <v>389</v>
       </c>
@@ -2970,47 +3124,58 @@
         <v>390</v>
       </c>
       <c r="C1" s="116" t="s">
-        <v>393</v>
-      </c>
-      <c r="D1" t="s">
-        <v>395</v>
-      </c>
-      <c r="E1" t="s">
-        <v>392</v>
-      </c>
-      <c r="F1" t="s">
-        <v>391</v>
-      </c>
-      <c r="G1" t="s">
-        <v>396</v>
-      </c>
-      <c r="H1" t="s">
-        <v>394</v>
-      </c>
-      <c r="I1" t="s">
-        <v>397</v>
-      </c>
-      <c r="J1" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>387</v>
       </c>
       <c r="B2" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C2" s="117"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>388</v>
       </c>
       <c r="B3" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C3" s="117"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="116" t="s">
+        <v>383</v>
+      </c>
+      <c r="B4" s="116" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="116" t="s">
+        <v>384</v>
+      </c>
+      <c r="B5" s="116" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="116" t="s">
+        <v>385</v>
+      </c>
+      <c r="B6" s="116" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="116" t="s">
+        <v>386</v>
+      </c>
+      <c r="B7" s="116" t="s">
+        <v>400</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3018,6 +3183,1337 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE180F16-E1DA-4BB3-8569-5BCDA49E36FB}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:N33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S1" sqref="S1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="3" width="9.109375" style="1"/>
+    <col min="4" max="4" width="37.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21" style="1" customWidth="1"/>
+    <col min="7" max="7" width="51.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="71.5546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="42.5546875" style="1" customWidth="1"/>
+    <col min="10" max="11" width="21" style="1" customWidth="1"/>
+    <col min="12" max="12" width="39.5546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="22.88671875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="21.44140625" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="11.44140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="28.8">
+      <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="144" hidden="1">
+      <c r="A2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2" s="15">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="100" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="101" t="s">
+        <v>232</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="M2" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="230.4" hidden="1">
+      <c r="A3" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="94"/>
+      <c r="C3" s="19">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="105" t="s">
+        <v>229</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" ht="230.4" hidden="1">
+      <c r="A4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="94"/>
+      <c r="C4" s="19">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="105" t="s">
+        <v>229</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" ht="244.8" hidden="1">
+      <c r="A5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="94" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="19">
+        <v>4</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="105" t="s">
+        <v>229</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" ht="230.4" hidden="1">
+      <c r="A6" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="94"/>
+      <c r="C6" s="19">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="J6" s="105" t="s">
+        <v>229</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" ht="201.6" hidden="1">
+      <c r="A7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C7" s="15">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H7" s="100" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="101" t="s">
+        <v>232</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="M7" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="316.8" hidden="1">
+      <c r="A8" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="15">
+        <v>7</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H8" s="100" t="s">
+        <v>87</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="101" t="s">
+        <v>232</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="99" t="s">
+        <v>89</v>
+      </c>
+      <c r="M8" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="316.8" hidden="1">
+      <c r="A9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C9" s="15">
+        <v>8</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" s="100" t="s">
+        <v>87</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="101" t="s">
+        <v>232</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M9" s="23" t="s">
+        <v>239</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="316.8">
+      <c r="A10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C10" s="15">
+        <v>9</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H10" s="100" t="s">
+        <v>87</v>
+      </c>
+      <c r="I10" s="103" t="s">
+        <v>241</v>
+      </c>
+      <c r="J10" s="102" t="s">
+        <v>80</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M10" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="N10" s="27" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="316.8" hidden="1">
+      <c r="A11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="15">
+        <v>10</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="101" t="s">
+        <v>232</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="L11" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M11" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="374.4" hidden="1">
+      <c r="A12" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C12" s="15">
+        <v>11</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="98" t="s">
+        <v>232</v>
+      </c>
+      <c r="K12" s="27"/>
+      <c r="L12" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M12" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="N12" s="104" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="374.4" hidden="1">
+      <c r="A13" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C13" s="15">
+        <v>12</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="101" t="s">
+        <v>232</v>
+      </c>
+      <c r="K13" s="3"/>
+      <c r="L13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M13" s="27" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="374.4" hidden="1">
+      <c r="A14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="15">
+        <v>13</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="101" t="s">
+        <v>232</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M14" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="374.4" hidden="1">
+      <c r="A15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C15" s="15">
+        <v>14</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="101" t="s">
+        <v>232</v>
+      </c>
+      <c r="K15" s="18"/>
+      <c r="L15" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M15" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="230.4" hidden="1">
+      <c r="B16" s="94"/>
+      <c r="C16" s="19">
+        <v>15</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="105" t="s">
+        <v>229</v>
+      </c>
+      <c r="K16" s="3"/>
+      <c r="L16" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M16" s="3"/>
+    </row>
+    <row r="17" spans="1:14" ht="230.4" hidden="1">
+      <c r="B17" s="94"/>
+      <c r="C17" s="19">
+        <v>16</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="105" t="s">
+        <v>229</v>
+      </c>
+      <c r="K17" s="3"/>
+      <c r="L17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M17" s="3"/>
+    </row>
+    <row r="18" spans="1:14" ht="230.4" hidden="1">
+      <c r="A18" s="11"/>
+      <c r="B18" s="94"/>
+      <c r="C18" s="19">
+        <v>17</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="105" t="s">
+        <v>229</v>
+      </c>
+      <c r="K18" s="3"/>
+      <c r="L18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M18" s="3"/>
+    </row>
+    <row r="19" spans="1:14" ht="244.8" hidden="1">
+      <c r="A19" s="11"/>
+      <c r="B19" s="94" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" s="19">
+        <v>18</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J19" s="105" t="s">
+        <v>229</v>
+      </c>
+      <c r="K19" s="3"/>
+      <c r="L19" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="M19" s="3"/>
+    </row>
+    <row r="20" spans="1:14" ht="230.4" hidden="1">
+      <c r="B20" s="94"/>
+      <c r="C20" s="19">
+        <v>19</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="105" t="s">
+        <v>229</v>
+      </c>
+      <c r="K20" s="3"/>
+      <c r="L20" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M20" s="3"/>
+    </row>
+    <row r="21" spans="1:14" ht="201.6" hidden="1">
+      <c r="A21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C21" s="15">
+        <v>20</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J21" s="101" t="s">
+        <v>232</v>
+      </c>
+      <c r="K21" s="24"/>
+      <c r="L21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="M21" s="27" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="201.6" hidden="1">
+      <c r="B22" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C22" s="15">
+        <v>21</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J22" s="101" t="s">
+        <v>232</v>
+      </c>
+      <c r="K22" s="3"/>
+      <c r="L22" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="M22" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="316.8" hidden="1">
+      <c r="B23" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C23" s="15">
+        <v>22</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J23" s="101" t="s">
+        <v>232</v>
+      </c>
+      <c r="K23" s="3"/>
+      <c r="L23" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M23" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="316.8" hidden="1">
+      <c r="A24" s="11"/>
+      <c r="B24" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C24" s="15">
+        <v>23</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I24" s="14"/>
+      <c r="J24" s="101" t="s">
+        <v>232</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M24" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="316.8" hidden="1">
+      <c r="A25" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C25" s="15">
+        <v>24</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J25" s="101" t="s">
+        <v>232</v>
+      </c>
+      <c r="K25" s="18"/>
+      <c r="L25" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M25" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="316.8" hidden="1">
+      <c r="B26" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C26" s="15">
+        <v>25</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J26" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="K26" s="3"/>
+      <c r="L26" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M26" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="N26"/>
+    </row>
+    <row r="27" spans="1:14" ht="374.4" hidden="1">
+      <c r="B27" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C27" s="15">
+        <v>26</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J27" s="101" t="s">
+        <v>232</v>
+      </c>
+      <c r="K27" s="3"/>
+      <c r="L27" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M27" s="27" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="374.4" hidden="1">
+      <c r="B28" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28" s="15">
+        <v>27</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J28" s="101" t="s">
+        <v>232</v>
+      </c>
+      <c r="K28" s="3"/>
+      <c r="L28" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M28" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="374.4" hidden="1">
+      <c r="A29" s="11"/>
+      <c r="B29" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C29" s="15">
+        <v>28</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J29" s="101" t="s">
+        <v>232</v>
+      </c>
+      <c r="K29" s="3"/>
+      <c r="L29" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M29" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="374.4" hidden="1">
+      <c r="A30" s="11"/>
+      <c r="B30" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C30" s="15">
+        <v>29</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J30" s="101" t="s">
+        <v>232</v>
+      </c>
+      <c r="K30" s="3"/>
+      <c r="L30" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M30" s="27" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="230.4" hidden="1">
+      <c r="B31" s="94"/>
+      <c r="C31" s="97">
+        <v>30</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I31" s="3"/>
+      <c r="J31" s="105" t="s">
+        <v>229</v>
+      </c>
+      <c r="K31" s="3"/>
+      <c r="L31" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M31" s="3"/>
+    </row>
+    <row r="32" spans="1:14" ht="230.4" hidden="1">
+      <c r="A32" s="11"/>
+      <c r="B32" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C32" s="15">
+        <v>31</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J32" s="101" t="s">
+        <v>232</v>
+      </c>
+      <c r="K32" s="3"/>
+      <c r="L32" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="M32" s="27" t="s">
+        <v>266</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="230.4" hidden="1">
+      <c r="A33" s="11"/>
+      <c r="B33" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C33" s="15">
+        <v>32</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J33" s="101" t="s">
+        <v>232</v>
+      </c>
+      <c r="K33" s="3"/>
+      <c r="L33" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="M33" s="23" t="s">
+        <v>268</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:M33" xr:uid="{DCB37448-7794-4D71-83D8-79D0F3D93892}">
+    <filterColumn colId="9">
+      <filters>
+        <filter val="Fallado"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{F54D3D39-555B-466A-B9C5-FC246C5F5B15}"/>
+    <hyperlink ref="L3:L5" r:id="rId2" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{2BE56167-CD4B-4F12-A70B-0F31AA292067}"/>
+    <hyperlink ref="L6" r:id="rId3" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{61DFD1AA-528A-4790-B293-945AE7E01231}"/>
+    <hyperlink ref="L7:L12" r:id="rId4" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{5B49D607-0BA1-4D10-A418-0A03B0FD88E0}"/>
+    <hyperlink ref="L16" r:id="rId5" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{39FDEEF1-D40D-4FF8-A44D-0822BE32A3F1}"/>
+    <hyperlink ref="L8" r:id="rId6" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{8E36D3F1-47FE-47F7-8F7A-3D2ED188E6E6}"/>
+    <hyperlink ref="L9" r:id="rId7" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{A98AF517-266A-4B8E-BBB8-9FFE4BCC26E4}"/>
+    <hyperlink ref="L10" r:id="rId8" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{67E0289D-6944-4362-B439-EFDBB2CB7159}"/>
+    <hyperlink ref="L11" r:id="rId9" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{BC426985-CAA8-4AEB-873B-C271CAF540A2}"/>
+    <hyperlink ref="L13" r:id="rId10" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{C7707C5D-86BB-4B58-8018-03A42F10E2B1}"/>
+    <hyperlink ref="L14" r:id="rId11" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{AACEADA1-DA1D-4A3D-B8B2-DE8C4C657755}"/>
+    <hyperlink ref="L15" r:id="rId12" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{2E2DE300-F6D1-49E5-9D44-9A238D663F76}"/>
+    <hyperlink ref="L17:L19" r:id="rId13" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{36CF93F6-9DC3-4D4A-AC44-3B051640E2B1}"/>
+    <hyperlink ref="L20" r:id="rId14" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{B94CFC9A-6EDF-48FB-9F05-1AE6629F978E}"/>
+    <hyperlink ref="L21:L27" r:id="rId15" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{0CDDE1F8-9626-4199-AF8C-1D7C0B743AFF}"/>
+    <hyperlink ref="L31" r:id="rId16" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{FAB99A4B-6FE0-401F-BD9C-38BC629D6204}"/>
+    <hyperlink ref="L23" r:id="rId17" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{20373B0F-10A7-46BD-83D3-2C16CE0781C8}"/>
+    <hyperlink ref="L24" r:id="rId18" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{980C2D28-ED2F-4AE4-89C9-23CED2D95206}"/>
+    <hyperlink ref="L25" r:id="rId19" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{38EC083F-B474-45BE-9A08-1AF11EB109F2}"/>
+    <hyperlink ref="L26" r:id="rId20" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{90596EF9-963E-4D80-9E9E-62D9AAB7FD31}"/>
+    <hyperlink ref="L28" r:id="rId21" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{5D92D9F1-DEDA-4090-B285-9405A39D2B14}"/>
+    <hyperlink ref="L29" r:id="rId22" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{B8A2C95D-79A7-48CE-BBD9-9FBDA07981B2}"/>
+    <hyperlink ref="L30" r:id="rId23" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{9952EAFE-7E46-4FBC-A97E-86E6A0D1CD34}"/>
+    <hyperlink ref="L32" r:id="rId24" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{CE025250-7C1F-4D77-8A75-359978202935}"/>
+    <hyperlink ref="L33" r:id="rId25" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{066B4A21-D070-40CF-B370-4736D8D3BD15}"/>
+    <hyperlink ref="M24" r:id="rId26" xr:uid="{4C4E5432-A969-47BF-B06D-1D8EC030D105}"/>
+    <hyperlink ref="M7" r:id="rId27" xr:uid="{7B46CFB9-C3F0-440A-9A17-F113601FA5F2}"/>
+    <hyperlink ref="M10" r:id="rId28" xr:uid="{FE79ACFA-514B-42E1-880A-544F21D906DD}"/>
+    <hyperlink ref="M2" r:id="rId29" xr:uid="{4918D815-F069-4AA7-976C-04FD321FD3D9}"/>
+    <hyperlink ref="M9" r:id="rId30" xr:uid="{B47E92A9-DCDE-40B5-8BF8-CA325FAA19CD}"/>
+    <hyperlink ref="M8" r:id="rId31" xr:uid="{3C1C2A90-BE62-4EF1-A230-4F8F9CB2D721}"/>
+    <hyperlink ref="N10" r:id="rId32" xr:uid="{48A23E75-481F-4B41-9CC5-C401DC5A9CA2}"/>
+    <hyperlink ref="M13" r:id="rId33" xr:uid="{C830212A-AEBC-4EC7-98C2-4B0FCE4BBF62}"/>
+    <hyperlink ref="M21" r:id="rId34" xr:uid="{7A6DF516-C44B-4209-91B2-07C1987C3420}"/>
+    <hyperlink ref="M12" r:id="rId35" xr:uid="{C02FBA2C-7DAF-4F63-9269-0BBEF0B07630}"/>
+    <hyperlink ref="M27" r:id="rId36" xr:uid="{4B45B753-9CC9-48CC-A188-FEBD5099EFF8}"/>
+    <hyperlink ref="M11" r:id="rId37" xr:uid="{188F3002-A368-4672-BADE-1CFCD8153E68}"/>
+    <hyperlink ref="M30" r:id="rId38" xr:uid="{B7F3D016-AF4D-4E4D-9E93-D5B494457A84}"/>
+    <hyperlink ref="M15" r:id="rId39" xr:uid="{5AF04AE5-AC0C-4F65-9283-21EB5A41951A}"/>
+    <hyperlink ref="M14" r:id="rId40" xr:uid="{B3F0AB56-A78B-4208-80FE-25BC9C101A0F}"/>
+    <hyperlink ref="M23" r:id="rId41" xr:uid="{B263E36A-E353-4F13-9D8A-100E8D206835}"/>
+    <hyperlink ref="M22" r:id="rId42" xr:uid="{09A06FEC-8471-48FF-810A-7EAE916989BD}"/>
+    <hyperlink ref="M26" r:id="rId43" xr:uid="{1DBBCD96-5879-4E8B-8CCE-B3DC9E52C042}"/>
+    <hyperlink ref="M25" r:id="rId44" xr:uid="{3BBAEC73-25C9-4D53-8F31-AC6C108A8BD9}"/>
+    <hyperlink ref="M29" r:id="rId45" xr:uid="{8B47F3CE-3A60-4BCC-B8A8-C0B907A86795}"/>
+    <hyperlink ref="M28" r:id="rId46" xr:uid="{B8785A92-9B80-444E-B239-EDA194ACFCC3}"/>
+    <hyperlink ref="M32" r:id="rId47" xr:uid="{ECAC17AD-1E1A-4E06-AAD8-99620C4252C7}"/>
+    <hyperlink ref="M33" r:id="rId48" xr:uid="{DE3B80FD-E607-4134-841E-8005649988FB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181D2DB1-0637-49E2-BE78-B1DD33F2D937}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N33"/>
@@ -4305,7 +5801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F1E6B3-AE0E-4F82-8CE5-818E954EB8E9}">
   <dimension ref="A1:N33"/>
   <sheetViews>
@@ -5569,7 +7065,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC121400-37A7-45CB-AB75-E80E51530A57}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M33"/>
@@ -6743,7 +8239,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6B80E1-D096-4AA5-AD9A-02A7B8F61FD8}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M33"/>
@@ -7931,7 +9427,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D869C7AD-B81B-46EF-9D92-1D8A4BF4B6FB}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M33"/>
@@ -9080,7 +10576,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB37448-7794-4D71-83D8-79D0F3D93892}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M33"/>
@@ -10223,7 +11719,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF491AA-1038-4BD9-85C2-55A46D475EEA}">
   <dimension ref="A1:AE16"/>
   <sheetViews>
@@ -11882,28 +13378,28 @@
     </row>
     <row r="3" spans="1:31" ht="15.75" customHeight="1">
       <c r="B3" s="44"/>
-      <c r="C3" s="134"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
-      <c r="H3" s="134"/>
-      <c r="I3" s="134"/>
-      <c r="J3" s="134"/>
-      <c r="K3" s="134"/>
-      <c r="L3" s="134"/>
-      <c r="M3" s="134"/>
-      <c r="N3" s="134"/>
-      <c r="O3" s="134"/>
-      <c r="P3" s="134"/>
-      <c r="Q3" s="134"/>
-      <c r="R3" s="134"/>
-      <c r="S3" s="134"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="118"/>
+      <c r="O3" s="118"/>
+      <c r="P3" s="118"/>
+      <c r="Q3" s="118"/>
+      <c r="R3" s="118"/>
+      <c r="S3" s="118"/>
       <c r="T3" s="45"/>
-      <c r="Y3" s="135"/>
-      <c r="Z3" s="135"/>
-      <c r="AA3" s="135"/>
-      <c r="AB3" s="135"/>
+      <c r="Y3" s="119"/>
+      <c r="Z3" s="119"/>
+      <c r="AA3" s="119"/>
+      <c r="AB3" s="119"/>
     </row>
     <row r="4" spans="1:31" ht="15" customHeight="1">
       <c r="B4" s="44"/>
@@ -11928,47 +13424,47 @@
     </row>
     <row r="5" spans="1:31" s="49" customFormat="1" ht="12.75" customHeight="1">
       <c r="B5" s="50"/>
-      <c r="C5" s="136" t="s">
+      <c r="C5" s="120" t="s">
         <v>358</v>
       </c>
-      <c r="D5" s="137"/>
-      <c r="E5" s="138"/>
-      <c r="F5" s="118" t="s">
+      <c r="D5" s="121"/>
+      <c r="E5" s="122"/>
+      <c r="F5" s="129" t="s">
         <v>359</v>
       </c>
-      <c r="G5" s="118" t="s">
+      <c r="G5" s="129" t="s">
         <v>360</v>
       </c>
-      <c r="H5" s="118" t="s">
+      <c r="H5" s="129" t="s">
         <v>361</v>
       </c>
-      <c r="I5" s="118" t="s">
+      <c r="I5" s="129" t="s">
         <v>362</v>
       </c>
-      <c r="J5" s="118" t="s">
+      <c r="J5" s="129" t="s">
         <v>363</v>
       </c>
-      <c r="K5" s="118" t="s">
+      <c r="K5" s="129" t="s">
         <v>364</v>
       </c>
-      <c r="L5" s="118" t="s">
+      <c r="L5" s="129" t="s">
         <v>365</v>
       </c>
-      <c r="M5" s="126" t="s">
+      <c r="M5" s="131" t="s">
         <v>366</v>
       </c>
-      <c r="N5" s="126" t="s">
+      <c r="N5" s="131" t="s">
         <v>367</v>
       </c>
-      <c r="O5" s="126" t="s">
+      <c r="O5" s="131" t="s">
         <v>368</v>
       </c>
-      <c r="P5" s="120" t="s">
+      <c r="P5" s="133" t="s">
         <v>369</v>
       </c>
-      <c r="Q5" s="121"/>
-      <c r="R5" s="121"/>
-      <c r="S5" s="122"/>
+      <c r="Q5" s="134"/>
+      <c r="R5" s="134"/>
+      <c r="S5" s="135"/>
       <c r="T5" s="51"/>
       <c r="U5" s="52"/>
       <c r="Y5" s="53"/>
@@ -11981,19 +13477,19 @@
     </row>
     <row r="6" spans="1:31" s="49" customFormat="1" ht="15" customHeight="1">
       <c r="B6" s="50"/>
-      <c r="C6" s="139"/>
-      <c r="D6" s="140"/>
-      <c r="E6" s="141"/>
-      <c r="F6" s="119"/>
-      <c r="G6" s="119"/>
-      <c r="H6" s="119"/>
-      <c r="I6" s="119"/>
-      <c r="J6" s="119"/>
-      <c r="K6" s="119"/>
-      <c r="L6" s="119"/>
-      <c r="M6" s="127"/>
-      <c r="N6" s="127"/>
-      <c r="O6" s="127"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="125"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="130"/>
+      <c r="H6" s="130"/>
+      <c r="I6" s="130"/>
+      <c r="J6" s="130"/>
+      <c r="K6" s="130"/>
+      <c r="L6" s="130"/>
+      <c r="M6" s="132"/>
+      <c r="N6" s="132"/>
+      <c r="O6" s="132"/>
       <c r="P6" s="54" t="s">
         <v>370</v>
       </c>
@@ -12018,9 +13514,9 @@
     </row>
     <row r="7" spans="1:31" s="56" customFormat="1" ht="15.75" customHeight="1">
       <c r="B7" s="57"/>
-      <c r="C7" s="142"/>
-      <c r="D7" s="143"/>
-      <c r="E7" s="144"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="127"/>
+      <c r="E7" s="128"/>
       <c r="F7" s="58">
         <f>F14</f>
         <v>32</v>
@@ -12131,49 +13627,49 @@
     </row>
     <row r="9" spans="1:31" s="49" customFormat="1" ht="15" customHeight="1">
       <c r="B9" s="50"/>
-      <c r="C9" s="128" t="s">
+      <c r="C9" s="136" t="s">
         <v>374</v>
       </c>
-      <c r="D9" s="130" t="s">
+      <c r="D9" s="138" t="s">
         <v>375</v>
       </c>
-      <c r="E9" s="131"/>
-      <c r="F9" s="132" t="s">
+      <c r="E9" s="139"/>
+      <c r="F9" s="140" t="s">
         <v>359</v>
       </c>
-      <c r="G9" s="118" t="s">
+      <c r="G9" s="129" t="s">
         <v>360</v>
       </c>
-      <c r="H9" s="118" t="s">
+      <c r="H9" s="129" t="s">
         <v>361</v>
       </c>
-      <c r="I9" s="118" t="s">
+      <c r="I9" s="129" t="s">
         <v>362</v>
       </c>
-      <c r="J9" s="118" t="s">
+      <c r="J9" s="129" t="s">
         <v>363</v>
       </c>
-      <c r="K9" s="118" t="s">
+      <c r="K9" s="129" t="s">
         <v>376</v>
       </c>
-      <c r="L9" s="118" t="s">
+      <c r="L9" s="129" t="s">
         <v>365</v>
       </c>
-      <c r="M9" s="126" t="s">
+      <c r="M9" s="131" t="s">
         <v>366</v>
       </c>
-      <c r="N9" s="126" t="s">
+      <c r="N9" s="131" t="s">
         <v>367</v>
       </c>
-      <c r="O9" s="126" t="s">
+      <c r="O9" s="131" t="s">
         <v>368</v>
       </c>
-      <c r="P9" s="120" t="s">
+      <c r="P9" s="133" t="s">
         <v>369</v>
       </c>
-      <c r="Q9" s="121"/>
-      <c r="R9" s="121"/>
-      <c r="S9" s="122"/>
+      <c r="Q9" s="134"/>
+      <c r="R9" s="134"/>
+      <c r="S9" s="135"/>
       <c r="T9" s="67"/>
       <c r="U9" s="68"/>
       <c r="Y9" s="55"/>
@@ -12186,23 +13682,23 @@
     </row>
     <row r="10" spans="1:31" s="49" customFormat="1" ht="15" customHeight="1">
       <c r="B10" s="50"/>
-      <c r="C10" s="129"/>
+      <c r="C10" s="137"/>
       <c r="D10" s="69" t="s">
         <v>377</v>
       </c>
       <c r="E10" s="70" t="s">
         <v>378</v>
       </c>
-      <c r="F10" s="133"/>
-      <c r="G10" s="119"/>
-      <c r="H10" s="119"/>
-      <c r="I10" s="119"/>
-      <c r="J10" s="119"/>
-      <c r="K10" s="119"/>
-      <c r="L10" s="119"/>
-      <c r="M10" s="127"/>
-      <c r="N10" s="127"/>
-      <c r="O10" s="127"/>
+      <c r="F10" s="141"/>
+      <c r="G10" s="130"/>
+      <c r="H10" s="130"/>
+      <c r="I10" s="130"/>
+      <c r="J10" s="130"/>
+      <c r="K10" s="130"/>
+      <c r="L10" s="130"/>
+      <c r="M10" s="132"/>
+      <c r="N10" s="132"/>
+      <c r="O10" s="132"/>
       <c r="P10" s="54" t="s">
         <v>370</v>
       </c>
@@ -12230,10 +13726,10 @@
       <c r="C11" s="71" t="s">
         <v>379</v>
       </c>
-      <c r="D11" s="123" t="s">
+      <c r="D11" s="142" t="s">
         <v>380</v>
       </c>
-      <c r="E11" s="123"/>
+      <c r="E11" s="142"/>
       <c r="F11" s="73">
         <f t="shared" ref="F11:L11" si="3">SUM(F12:F13)</f>
         <v>32</v>
@@ -12305,8 +13801,8 @@
       <c r="C12" s="78" t="s">
         <v>381</v>
       </c>
-      <c r="D12" s="124"/>
-      <c r="E12" s="124"/>
+      <c r="D12" s="143"/>
+      <c r="E12" s="143"/>
       <c r="F12" s="79">
         <v>16</v>
       </c>
@@ -12368,8 +13864,8 @@
       <c r="C13" s="78" t="s">
         <v>382</v>
       </c>
-      <c r="D13" s="124"/>
-      <c r="E13" s="124"/>
+      <c r="D13" s="143"/>
+      <c r="E13" s="143"/>
       <c r="F13" s="79">
         <v>16</v>
       </c>
@@ -12523,12 +14019,28 @@
       <c r="T15" s="92"/>
     </row>
     <row r="16" spans="1:31">
-      <c r="F16" s="125"/>
-      <c r="G16" s="125"/>
-      <c r="H16" s="125"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="P9:S9"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
     <mergeCell ref="C3:S3"/>
     <mergeCell ref="Y3:AB3"/>
     <mergeCell ref="C5:E7"/>
@@ -12543,22 +14055,6 @@
     <mergeCell ref="N5:N6"/>
     <mergeCell ref="O5:O6"/>
     <mergeCell ref="P5:S5"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="P9:S9"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
   </mergeCells>
   <conditionalFormatting sqref="U11:X14">
     <cfRule type="iconSet" priority="2">
@@ -12593,101 +14089,742 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC98DD0-04DF-46E2-AE89-603FE9DF8BD7}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="41.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="116" t="s">
-        <v>383</v>
-      </c>
-      <c r="B1" s="116" t="s">
-        <v>402</v>
-      </c>
-      <c r="C1" s="145"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="116"/>
-      <c r="J1" s="116"/>
-    </row>
-    <row r="2" spans="1:10">
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C1" t="s">
+        <v>397</v>
+      </c>
+      <c r="D1" s="116" t="s">
+        <v>393</v>
+      </c>
+      <c r="E1" s="116" t="s">
+        <v>409</v>
+      </c>
+      <c r="F1" s="116" t="s">
+        <v>416</v>
+      </c>
+      <c r="G1" t="s">
+        <v>395</v>
+      </c>
+      <c r="H1" t="s">
+        <v>392</v>
+      </c>
+      <c r="I1" t="s">
+        <v>391</v>
+      </c>
+      <c r="J1" t="s">
+        <v>396</v>
+      </c>
+      <c r="K1" t="s">
+        <v>394</v>
+      </c>
+      <c r="L1" t="s">
+        <v>449</v>
+      </c>
+      <c r="M1" t="s">
+        <v>439</v>
+      </c>
+      <c r="N1" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="116" t="s">
         <v>384</v>
       </c>
       <c r="B2" s="116" t="s">
+        <v>399</v>
+      </c>
+      <c r="C2" s="116" t="s">
+        <v>413</v>
+      </c>
+      <c r="D2" s="146" t="s">
         <v>402</v>
       </c>
-      <c r="C2" s="145"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="E2" s="146" t="s">
+        <v>410</v>
+      </c>
+      <c r="F2" s="146" t="s">
+        <v>417</v>
+      </c>
+      <c r="G2" t="s">
+        <v>415</v>
+      </c>
+      <c r="H2" s="146" t="s">
+        <v>437</v>
+      </c>
+      <c r="I2">
+        <v>12</v>
+      </c>
+      <c r="J2">
+        <v>24</v>
+      </c>
+      <c r="K2">
+        <v>546</v>
+      </c>
+      <c r="L2" t="s">
+        <v>440</v>
+      </c>
+      <c r="M2" t="s">
+        <v>450</v>
+      </c>
+      <c r="N2" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="116" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B3" s="116" t="s">
+        <v>399</v>
+      </c>
+      <c r="C3" s="116" t="s">
+        <v>413</v>
+      </c>
+      <c r="D3" s="146" t="s">
         <v>402</v>
       </c>
-      <c r="C3" s="145">
-        <v>4111111111111110</v>
-      </c>
-      <c r="D3" s="116"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="116"/>
-      <c r="G3" s="116"/>
-      <c r="H3" s="116"/>
-      <c r="I3" s="116" t="s">
+      <c r="E3" s="146" t="s">
+        <v>410</v>
+      </c>
+      <c r="F3" s="146" t="s">
+        <v>418</v>
+      </c>
+      <c r="G3" t="s">
+        <v>415</v>
+      </c>
+      <c r="H3" s="146" t="s">
+        <v>437</v>
+      </c>
+      <c r="I3">
+        <v>11</v>
+      </c>
+      <c r="J3">
+        <v>25</v>
+      </c>
+      <c r="K3">
+        <v>546</v>
+      </c>
+      <c r="L3" t="s">
+        <v>441</v>
+      </c>
+      <c r="M3" t="s">
+        <v>451</v>
+      </c>
+      <c r="N3" s="145" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="116" t="s">
+        <v>384</v>
+      </c>
+      <c r="B4" s="116" t="s">
+        <v>399</v>
+      </c>
+      <c r="C4" s="116" t="s">
+        <v>414</v>
+      </c>
+      <c r="D4" s="146" t="s">
+        <v>412</v>
+      </c>
+      <c r="E4" s="146" t="s">
+        <v>411</v>
+      </c>
+      <c r="F4" s="146" t="s">
+        <v>417</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4" s="146" t="s">
+        <v>437</v>
+      </c>
+      <c r="I4">
+        <v>12</v>
+      </c>
+      <c r="J4">
+        <v>24</v>
+      </c>
+      <c r="K4">
+        <v>546</v>
+      </c>
+      <c r="L4" t="s">
+        <v>446</v>
+      </c>
+      <c r="M4" t="s">
+        <v>452</v>
+      </c>
+      <c r="N4" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="116" t="s">
+        <v>384</v>
+      </c>
+      <c r="B5" s="116" t="s">
+        <v>399</v>
+      </c>
+      <c r="C5" s="116" t="s">
+        <v>414</v>
+      </c>
+      <c r="D5" s="146" t="s">
+        <v>412</v>
+      </c>
+      <c r="E5" s="146" t="s">
+        <v>411</v>
+      </c>
+      <c r="F5" s="146" t="s">
+        <v>418</v>
+      </c>
+      <c r="G5">
+        <v>12</v>
+      </c>
+      <c r="H5" s="146" t="s">
+        <v>437</v>
+      </c>
+      <c r="I5">
+        <v>11</v>
+      </c>
+      <c r="J5">
+        <v>25</v>
+      </c>
+      <c r="K5">
+        <v>546</v>
+      </c>
+      <c r="L5" t="s">
+        <v>447</v>
+      </c>
+      <c r="M5" s="145" t="s">
+        <v>452</v>
+      </c>
+      <c r="N5" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="116" t="s">
+        <v>384</v>
+      </c>
+      <c r="B6" s="116" t="s">
+        <v>399</v>
+      </c>
+      <c r="C6" s="116" t="s">
+        <v>414</v>
+      </c>
+      <c r="D6" s="146" t="s">
+        <v>412</v>
+      </c>
+      <c r="E6" s="146" t="s">
+        <v>411</v>
+      </c>
+      <c r="F6" s="146" t="s">
+        <v>160</v>
+      </c>
+      <c r="G6">
+        <v>12</v>
+      </c>
+      <c r="H6" s="146" t="s">
+        <v>437</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>30</v>
+      </c>
+      <c r="K6">
+        <v>546</v>
+      </c>
+      <c r="L6" t="s">
+        <v>442</v>
+      </c>
+      <c r="M6" s="145" t="s">
+        <v>452</v>
+      </c>
+      <c r="N6" s="145" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="116" t="s">
+        <v>384</v>
+      </c>
+      <c r="B7" s="116" t="s">
+        <v>399</v>
+      </c>
+      <c r="C7" s="116" t="s">
+        <v>415</v>
+      </c>
+      <c r="D7" s="146" t="s">
+        <v>403</v>
+      </c>
+      <c r="E7" s="116" t="s">
+        <v>415</v>
+      </c>
+      <c r="F7" s="146" t="s">
+        <v>406</v>
+      </c>
+      <c r="G7" t="s">
+        <v>415</v>
+      </c>
+      <c r="H7" s="146" t="s">
+        <v>437</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>30</v>
+      </c>
+      <c r="K7">
+        <v>546</v>
+      </c>
+      <c r="L7" t="s">
+        <v>442</v>
+      </c>
+      <c r="M7" s="145" t="s">
+        <v>452</v>
+      </c>
+      <c r="N7" s="145" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="116" t="s">
+        <v>384</v>
+      </c>
+      <c r="B8" s="116" t="s">
+        <v>399</v>
+      </c>
+      <c r="C8" s="116" t="s">
+        <v>415</v>
+      </c>
+      <c r="D8" s="146" t="s">
+        <v>404</v>
+      </c>
+      <c r="E8" s="116" t="s">
+        <v>415</v>
+      </c>
+      <c r="F8" s="146" t="s">
+        <v>405</v>
+      </c>
+      <c r="G8" t="s">
+        <v>415</v>
+      </c>
+      <c r="H8" s="146" t="s">
+        <v>437</v>
+      </c>
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8">
+        <v>30</v>
+      </c>
+      <c r="K8">
+        <v>546</v>
+      </c>
+      <c r="L8" t="s">
+        <v>442</v>
+      </c>
+      <c r="M8" s="145" t="s">
+        <v>452</v>
+      </c>
+      <c r="N8" s="145" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="116" t="s">
+        <v>384</v>
+      </c>
+      <c r="B9" s="116" t="s">
+        <v>399</v>
+      </c>
+      <c r="C9" s="116" t="s">
+        <v>415</v>
+      </c>
+      <c r="D9" s="146" t="s">
+        <v>408</v>
+      </c>
+      <c r="E9" s="116" t="s">
+        <v>415</v>
+      </c>
+      <c r="F9" s="146" t="s">
+        <v>407</v>
+      </c>
+      <c r="G9" t="s">
+        <v>415</v>
+      </c>
+      <c r="H9" s="146" t="s">
+        <v>437</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <v>30</v>
+      </c>
+      <c r="K9">
+        <v>546</v>
+      </c>
+      <c r="L9" t="s">
+        <v>442</v>
+      </c>
+      <c r="M9" s="145" t="s">
+        <v>452</v>
+      </c>
+      <c r="N9" s="145" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="116" t="s">
+        <v>383</v>
+      </c>
+      <c r="B10" s="116" t="s">
+        <v>399</v>
+      </c>
+      <c r="C10" s="116" t="s">
         <v>398</v>
       </c>
-      <c r="J3" s="116"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="116" t="s">
-        <v>386</v>
-      </c>
-      <c r="B4" s="116" t="s">
-        <v>403</v>
-      </c>
-      <c r="C4" s="145">
-        <v>5105105105105100</v>
-      </c>
-      <c r="D4" s="116"/>
-      <c r="E4" s="116"/>
-      <c r="F4" s="116"/>
-      <c r="G4" s="116"/>
-      <c r="H4" s="116"/>
-      <c r="I4" s="116" t="s">
+      <c r="D10" s="146" t="s">
+        <v>420</v>
+      </c>
+      <c r="E10" s="147" t="s">
+        <v>419</v>
+      </c>
+      <c r="F10" s="146" t="s">
+        <v>417</v>
+      </c>
+      <c r="G10" t="s">
+        <v>415</v>
+      </c>
+      <c r="H10" s="146" t="s">
+        <v>437</v>
+      </c>
+      <c r="I10">
+        <v>12</v>
+      </c>
+      <c r="J10">
+        <v>24</v>
+      </c>
+      <c r="K10">
+        <v>546</v>
+      </c>
+      <c r="L10" t="s">
+        <v>442</v>
+      </c>
+      <c r="M10" s="145" t="s">
+        <v>452</v>
+      </c>
+      <c r="N10" s="145" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="116" t="s">
+        <v>383</v>
+      </c>
+      <c r="B11" s="116" t="s">
         <v>399</v>
       </c>
-      <c r="J4" s="116"/>
+      <c r="C11" s="116" t="s">
+        <v>398</v>
+      </c>
+      <c r="D11" s="146" t="s">
+        <v>421</v>
+      </c>
+      <c r="E11" s="147" t="s">
+        <v>419</v>
+      </c>
+      <c r="F11" s="146" t="s">
+        <v>418</v>
+      </c>
+      <c r="G11" t="s">
+        <v>415</v>
+      </c>
+      <c r="H11" s="146" t="s">
+        <v>437</v>
+      </c>
+      <c r="I11">
+        <v>11</v>
+      </c>
+      <c r="J11">
+        <v>25</v>
+      </c>
+      <c r="K11">
+        <v>546</v>
+      </c>
+      <c r="L11" t="s">
+        <v>442</v>
+      </c>
+      <c r="M11" s="145" t="s">
+        <v>452</v>
+      </c>
+      <c r="N11" s="145" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="116" t="s">
+        <v>383</v>
+      </c>
+      <c r="B12" s="116" t="s">
+        <v>399</v>
+      </c>
+      <c r="C12" s="116" t="s">
+        <v>398</v>
+      </c>
+      <c r="D12" s="146" t="s">
+        <v>422</v>
+      </c>
+      <c r="E12" s="147" t="s">
+        <v>419</v>
+      </c>
+      <c r="F12" s="146" t="s">
+        <v>406</v>
+      </c>
+      <c r="G12" t="s">
+        <v>415</v>
+      </c>
+      <c r="H12" s="146" t="s">
+        <v>437</v>
+      </c>
+      <c r="I12">
+        <v>9</v>
+      </c>
+      <c r="J12">
+        <v>30</v>
+      </c>
+      <c r="K12">
+        <v>546</v>
+      </c>
+      <c r="L12" t="s">
+        <v>442</v>
+      </c>
+      <c r="M12" s="145" t="s">
+        <v>452</v>
+      </c>
+      <c r="N12" s="145" t="s">
+        <v>443</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC840DFD-BF02-410F-B2FC-5DCEDA6A1019}">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="61.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>424</v>
+      </c>
+      <c r="B2" s="95" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>424</v>
+      </c>
+      <c r="B3" s="95" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>424</v>
+      </c>
+      <c r="B4" s="95" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>424</v>
+      </c>
+      <c r="B5" s="95" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>424</v>
+      </c>
+      <c r="B6" s="95" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>424</v>
+      </c>
+      <c r="B7" s="95" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>424</v>
+      </c>
+      <c r="B8" s="95" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>424</v>
+      </c>
+      <c r="B9" s="95" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>425</v>
+      </c>
+      <c r="B10" s="95" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>425</v>
+      </c>
+      <c r="B11" s="95" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>425</v>
+      </c>
+      <c r="B12" s="95" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>425</v>
+      </c>
+      <c r="B13" s="95" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>425</v>
+      </c>
+      <c r="B14" s="95" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>425</v>
+      </c>
+      <c r="B15" s="95" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>425</v>
+      </c>
+      <c r="B16" s="95" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>425</v>
+      </c>
+      <c r="B17" s="95" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>425</v>
+      </c>
+      <c r="B18" s="95" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>425</v>
+      </c>
+      <c r="B19" s="95" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>425</v>
+      </c>
+      <c r="B20" s="95" t="s">
+        <v>427</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703084B0-7020-4228-BA63-87A3B98F18A3}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1"/>
@@ -13210,7 +15347,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{276724DB-1A94-4063-A318-86352BC79020}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N33"/>
@@ -14543,7 +16680,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FB9472-2E2F-4C8E-8379-6B5FA0E476A2}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N33"/>
@@ -15838,7 +17975,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDB9C14-3C91-42A1-B5CD-64E20BDBD4B5}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N33"/>
@@ -17071,7 +19208,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31CE0FA-6A3C-4645-AE25-E75B2D5D9895}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N33"/>
@@ -18285,7 +20422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F87DEE-8A67-4F56-AB92-709EFA44E565}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N33"/>
@@ -19597,1337 +21734,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE180F16-E1DA-4BB3-8569-5BCDA49E36FB}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:N33"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S1" sqref="S1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2" max="3" width="9.109375" style="1"/>
-    <col min="4" max="4" width="37.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="40" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21" style="1" customWidth="1"/>
-    <col min="7" max="7" width="51.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="71.5546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="42.5546875" style="1" customWidth="1"/>
-    <col min="10" max="11" width="21" style="1" customWidth="1"/>
-    <col min="12" max="12" width="39.5546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="22.88671875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="21.44140625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.44140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="28.8">
-      <c r="B1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="N1" s="30" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="144" hidden="1">
-      <c r="A2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C2" s="15">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H2" s="100" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="101" t="s">
-        <v>232</v>
-      </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="M2" s="23" t="s">
-        <v>233</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="230.4" hidden="1">
-      <c r="A3" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="94"/>
-      <c r="C3" s="19">
-        <v>2</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="105" t="s">
-        <v>229</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:14" ht="230.4" hidden="1">
-      <c r="A4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="94"/>
-      <c r="C4" s="19">
-        <v>3</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="105" t="s">
-        <v>229</v>
-      </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="M4" s="3"/>
-    </row>
-    <row r="5" spans="1:14" ht="244.8" hidden="1">
-      <c r="A5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="94" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="19">
-        <v>4</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="105" t="s">
-        <v>229</v>
-      </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="M5" s="3"/>
-    </row>
-    <row r="6" spans="1:14" ht="230.4" hidden="1">
-      <c r="A6" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="94"/>
-      <c r="C6" s="19">
-        <v>5</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="J6" s="105" t="s">
-        <v>229</v>
-      </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="M6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" ht="201.6" hidden="1">
-      <c r="A7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C7" s="15">
-        <v>6</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H7" s="100" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="101" t="s">
-        <v>232</v>
-      </c>
-      <c r="K7" s="3"/>
-      <c r="L7" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="M7" s="27" t="s">
-        <v>235</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="316.8" hidden="1">
-      <c r="A8" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" s="15">
-        <v>7</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H8" s="100" t="s">
-        <v>87</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" s="101" t="s">
-        <v>232</v>
-      </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="99" t="s">
-        <v>89</v>
-      </c>
-      <c r="M8" s="17" t="s">
-        <v>237</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="316.8" hidden="1">
-      <c r="A9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C9" s="15">
-        <v>8</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H9" s="100" t="s">
-        <v>87</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J9" s="101" t="s">
-        <v>232</v>
-      </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M9" s="23" t="s">
-        <v>239</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="316.8">
-      <c r="A10" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C10" s="15">
-        <v>9</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H10" s="100" t="s">
-        <v>87</v>
-      </c>
-      <c r="I10" s="103" t="s">
-        <v>241</v>
-      </c>
-      <c r="J10" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M10" s="27" t="s">
-        <v>243</v>
-      </c>
-      <c r="N10" s="27" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="316.8" hidden="1">
-      <c r="A11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" s="15">
-        <v>10</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" s="101" t="s">
-        <v>232</v>
-      </c>
-      <c r="K11" s="3"/>
-      <c r="L11" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M11" s="17" t="s">
-        <v>245</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="374.4" hidden="1">
-      <c r="A12" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C12" s="15">
-        <v>11</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="98" t="s">
-        <v>232</v>
-      </c>
-      <c r="K12" s="27"/>
-      <c r="L12" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M12" s="23" t="s">
-        <v>212</v>
-      </c>
-      <c r="N12" s="104" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="374.4" hidden="1">
-      <c r="A13" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C13" s="15">
-        <v>12</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J13" s="101" t="s">
-        <v>232</v>
-      </c>
-      <c r="K13" s="3"/>
-      <c r="L13" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M13" s="27" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="374.4" hidden="1">
-      <c r="A14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C14" s="15">
-        <v>13</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J14" s="101" t="s">
-        <v>232</v>
-      </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M14" s="27" t="s">
-        <v>249</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="374.4" hidden="1">
-      <c r="A15" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C15" s="15">
-        <v>14</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J15" s="101" t="s">
-        <v>232</v>
-      </c>
-      <c r="K15" s="18"/>
-      <c r="L15" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M15" s="23" t="s">
-        <v>215</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="230.4" hidden="1">
-      <c r="B16" s="94"/>
-      <c r="C16" s="19">
-        <v>15</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="105" t="s">
-        <v>229</v>
-      </c>
-      <c r="K16" s="3"/>
-      <c r="L16" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="M16" s="3"/>
-    </row>
-    <row r="17" spans="1:14" ht="230.4" hidden="1">
-      <c r="B17" s="94"/>
-      <c r="C17" s="19">
-        <v>16</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="105" t="s">
-        <v>229</v>
-      </c>
-      <c r="K17" s="3"/>
-      <c r="L17" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="M17" s="3"/>
-    </row>
-    <row r="18" spans="1:14" ht="230.4" hidden="1">
-      <c r="A18" s="11"/>
-      <c r="B18" s="94"/>
-      <c r="C18" s="19">
-        <v>17</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="105" t="s">
-        <v>229</v>
-      </c>
-      <c r="K18" s="3"/>
-      <c r="L18" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="M18" s="3"/>
-    </row>
-    <row r="19" spans="1:14" ht="244.8" hidden="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="94" t="s">
-        <v>116</v>
-      </c>
-      <c r="C19" s="19">
-        <v>18</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="J19" s="105" t="s">
-        <v>229</v>
-      </c>
-      <c r="K19" s="3"/>
-      <c r="L19" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="M19" s="3"/>
-    </row>
-    <row r="20" spans="1:14" ht="230.4" hidden="1">
-      <c r="B20" s="94"/>
-      <c r="C20" s="19">
-        <v>19</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="105" t="s">
-        <v>229</v>
-      </c>
-      <c r="K20" s="3"/>
-      <c r="L20" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="M20" s="3"/>
-    </row>
-    <row r="21" spans="1:14" ht="201.6" hidden="1">
-      <c r="A21" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C21" s="15">
-        <v>20</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J21" s="101" t="s">
-        <v>232</v>
-      </c>
-      <c r="K21" s="24"/>
-      <c r="L21" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="M21" s="27" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="201.6" hidden="1">
-      <c r="B22" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C22" s="15">
-        <v>21</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J22" s="101" t="s">
-        <v>232</v>
-      </c>
-      <c r="K22" s="3"/>
-      <c r="L22" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="M22" s="27" t="s">
-        <v>253</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="316.8" hidden="1">
-      <c r="B23" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C23" s="15">
-        <v>22</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J23" s="101" t="s">
-        <v>232</v>
-      </c>
-      <c r="K23" s="3"/>
-      <c r="L23" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M23" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="316.8" hidden="1">
-      <c r="A24" s="11"/>
-      <c r="B24" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C24" s="15">
-        <v>23</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I24" s="14"/>
-      <c r="J24" s="101" t="s">
-        <v>232</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M24" s="27" t="s">
-        <v>257</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="316.8" hidden="1">
-      <c r="A25" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C25" s="15">
-        <v>24</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J25" s="101" t="s">
-        <v>232</v>
-      </c>
-      <c r="K25" s="18"/>
-      <c r="L25" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M25" s="27" t="s">
-        <v>259</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="316.8" hidden="1">
-      <c r="B26" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C26" s="15">
-        <v>25</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J26" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="K26" s="3"/>
-      <c r="L26" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M26" s="23" t="s">
-        <v>261</v>
-      </c>
-      <c r="N26"/>
-    </row>
-    <row r="27" spans="1:14" ht="374.4" hidden="1">
-      <c r="B27" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C27" s="15">
-        <v>26</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J27" s="101" t="s">
-        <v>232</v>
-      </c>
-      <c r="K27" s="3"/>
-      <c r="L27" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M27" s="27" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="374.4" hidden="1">
-      <c r="B28" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C28" s="15">
-        <v>27</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J28" s="101" t="s">
-        <v>232</v>
-      </c>
-      <c r="K28" s="3"/>
-      <c r="L28" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M28" s="27" t="s">
-        <v>263</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="374.4" hidden="1">
-      <c r="A29" s="11"/>
-      <c r="B29" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C29" s="15">
-        <v>28</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J29" s="101" t="s">
-        <v>232</v>
-      </c>
-      <c r="K29" s="3"/>
-      <c r="L29" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M29" s="23" t="s">
-        <v>225</v>
-      </c>
-      <c r="N29" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="374.4" hidden="1">
-      <c r="A30" s="11"/>
-      <c r="B30" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C30" s="15">
-        <v>29</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J30" s="101" t="s">
-        <v>232</v>
-      </c>
-      <c r="K30" s="3"/>
-      <c r="L30" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M30" s="27" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" ht="230.4" hidden="1">
-      <c r="B31" s="94"/>
-      <c r="C31" s="97">
-        <v>30</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I31" s="3"/>
-      <c r="J31" s="105" t="s">
-        <v>229</v>
-      </c>
-      <c r="K31" s="3"/>
-      <c r="L31" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="M31" s="3"/>
-    </row>
-    <row r="32" spans="1:14" ht="230.4" hidden="1">
-      <c r="A32" s="11"/>
-      <c r="B32" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C32" s="15">
-        <v>31</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J32" s="101" t="s">
-        <v>232</v>
-      </c>
-      <c r="K32" s="3"/>
-      <c r="L32" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="M32" s="27" t="s">
-        <v>266</v>
-      </c>
-      <c r="N32" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" ht="230.4" hidden="1">
-      <c r="A33" s="11"/>
-      <c r="B33" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C33" s="15">
-        <v>32</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J33" s="101" t="s">
-        <v>232</v>
-      </c>
-      <c r="K33" s="3"/>
-      <c r="L33" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="M33" s="23" t="s">
-        <v>268</v>
-      </c>
-      <c r="N33" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:M33" xr:uid="{DCB37448-7794-4D71-83D8-79D0F3D93892}">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="Fallado"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{F54D3D39-555B-466A-B9C5-FC246C5F5B15}"/>
-    <hyperlink ref="L3:L5" r:id="rId2" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{2BE56167-CD4B-4F12-A70B-0F31AA292067}"/>
-    <hyperlink ref="L6" r:id="rId3" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{61DFD1AA-528A-4790-B293-945AE7E01231}"/>
-    <hyperlink ref="L7:L12" r:id="rId4" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{5B49D607-0BA1-4D10-A418-0A03B0FD88E0}"/>
-    <hyperlink ref="L16" r:id="rId5" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{39FDEEF1-D40D-4FF8-A44D-0822BE32A3F1}"/>
-    <hyperlink ref="L8" r:id="rId6" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{8E36D3F1-47FE-47F7-8F7A-3D2ED188E6E6}"/>
-    <hyperlink ref="L9" r:id="rId7" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{A98AF517-266A-4B8E-BBB8-9FFE4BCC26E4}"/>
-    <hyperlink ref="L10" r:id="rId8" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{67E0289D-6944-4362-B439-EFDBB2CB7159}"/>
-    <hyperlink ref="L11" r:id="rId9" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{BC426985-CAA8-4AEB-873B-C271CAF540A2}"/>
-    <hyperlink ref="L13" r:id="rId10" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{C7707C5D-86BB-4B58-8018-03A42F10E2B1}"/>
-    <hyperlink ref="L14" r:id="rId11" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{AACEADA1-DA1D-4A3D-B8B2-DE8C4C657755}"/>
-    <hyperlink ref="L15" r:id="rId12" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{2E2DE300-F6D1-49E5-9D44-9A238D663F76}"/>
-    <hyperlink ref="L17:L19" r:id="rId13" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{36CF93F6-9DC3-4D4A-AC44-3B051640E2B1}"/>
-    <hyperlink ref="L20" r:id="rId14" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{B94CFC9A-6EDF-48FB-9F05-1AE6629F978E}"/>
-    <hyperlink ref="L21:L27" r:id="rId15" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{0CDDE1F8-9626-4199-AF8C-1D7C0B743AFF}"/>
-    <hyperlink ref="L31" r:id="rId16" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{FAB99A4B-6FE0-401F-BD9C-38BC629D6204}"/>
-    <hyperlink ref="L23" r:id="rId17" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{20373B0F-10A7-46BD-83D3-2C16CE0781C8}"/>
-    <hyperlink ref="L24" r:id="rId18" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{980C2D28-ED2F-4AE4-89C9-23CED2D95206}"/>
-    <hyperlink ref="L25" r:id="rId19" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{38EC083F-B474-45BE-9A08-1AF11EB109F2}"/>
-    <hyperlink ref="L26" r:id="rId20" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{90596EF9-963E-4D80-9E9E-62D9AAB7FD31}"/>
-    <hyperlink ref="L28" r:id="rId21" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{5D92D9F1-DEDA-4090-B285-9405A39D2B14}"/>
-    <hyperlink ref="L29" r:id="rId22" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{B8A2C95D-79A7-48CE-BBD9-9FBDA07981B2}"/>
-    <hyperlink ref="L30" r:id="rId23" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{9952EAFE-7E46-4FBC-A97E-86E6A0D1CD34}"/>
-    <hyperlink ref="L32" r:id="rId24" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{CE025250-7C1F-4D77-8A75-359978202935}"/>
-    <hyperlink ref="L33" r:id="rId25" display="https://app.clickup.com/t/8499449/APP-250" xr:uid="{066B4A21-D070-40CF-B370-4736D8D3BD15}"/>
-    <hyperlink ref="M24" r:id="rId26" xr:uid="{4C4E5432-A969-47BF-B06D-1D8EC030D105}"/>
-    <hyperlink ref="M7" r:id="rId27" xr:uid="{7B46CFB9-C3F0-440A-9A17-F113601FA5F2}"/>
-    <hyperlink ref="M10" r:id="rId28" xr:uid="{FE79ACFA-514B-42E1-880A-544F21D906DD}"/>
-    <hyperlink ref="M2" r:id="rId29" xr:uid="{4918D815-F069-4AA7-976C-04FD321FD3D9}"/>
-    <hyperlink ref="M9" r:id="rId30" xr:uid="{B47E92A9-DCDE-40B5-8BF8-CA325FAA19CD}"/>
-    <hyperlink ref="M8" r:id="rId31" xr:uid="{3C1C2A90-BE62-4EF1-A230-4F8F9CB2D721}"/>
-    <hyperlink ref="N10" r:id="rId32" xr:uid="{48A23E75-481F-4B41-9CC5-C401DC5A9CA2}"/>
-    <hyperlink ref="M13" r:id="rId33" xr:uid="{C830212A-AEBC-4EC7-98C2-4B0FCE4BBF62}"/>
-    <hyperlink ref="M21" r:id="rId34" xr:uid="{7A6DF516-C44B-4209-91B2-07C1987C3420}"/>
-    <hyperlink ref="M12" r:id="rId35" xr:uid="{C02FBA2C-7DAF-4F63-9269-0BBEF0B07630}"/>
-    <hyperlink ref="M27" r:id="rId36" xr:uid="{4B45B753-9CC9-48CC-A188-FEBD5099EFF8}"/>
-    <hyperlink ref="M11" r:id="rId37" xr:uid="{188F3002-A368-4672-BADE-1CFCD8153E68}"/>
-    <hyperlink ref="M30" r:id="rId38" xr:uid="{B7F3D016-AF4D-4E4D-9E93-D5B494457A84}"/>
-    <hyperlink ref="M15" r:id="rId39" xr:uid="{5AF04AE5-AC0C-4F65-9283-21EB5A41951A}"/>
-    <hyperlink ref="M14" r:id="rId40" xr:uid="{B3F0AB56-A78B-4208-80FE-25BC9C101A0F}"/>
-    <hyperlink ref="M23" r:id="rId41" xr:uid="{B263E36A-E353-4F13-9D8A-100E8D206835}"/>
-    <hyperlink ref="M22" r:id="rId42" xr:uid="{09A06FEC-8471-48FF-810A-7EAE916989BD}"/>
-    <hyperlink ref="M26" r:id="rId43" xr:uid="{1DBBCD96-5879-4E8B-8CCE-B3DC9E52C042}"/>
-    <hyperlink ref="M25" r:id="rId44" xr:uid="{3BBAEC73-25C9-4D53-8F31-AC6C108A8BD9}"/>
-    <hyperlink ref="M29" r:id="rId45" xr:uid="{8B47F3CE-3A60-4BCC-B8A8-C0B907A86795}"/>
-    <hyperlink ref="M28" r:id="rId46" xr:uid="{B8785A92-9B80-444E-B239-EDA194ACFCC3}"/>
-    <hyperlink ref="M32" r:id="rId47" xr:uid="{ECAC17AD-1E1A-4E06-AAD8-99620C4252C7}"/>
-    <hyperlink ref="M33" r:id="rId48" xr:uid="{DE3B80FD-E607-4134-841E-8005649988FB}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -20938,6 +21744,19 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="07fe17d8-c930-4881-be9b-3b241872ecf2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a516c34c-5f40-4b9f-bc5a-0e3bcef9c56f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001281E93D4CD8AF4592CEAE70F49402AE" ma:contentTypeVersion="19" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="bc27ca239ee5364de882bf49db749c36">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="07fe17d8-c930-4881-be9b-3b241872ecf2" xmlns:ns3="a516c34c-5f40-4b9f-bc5a-0e3bcef9c56f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dfd02d4500181950e6ebedca310b1d56" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -21195,19 +22014,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="07fe17d8-c930-4881-be9b-3b241872ecf2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a516c34c-5f40-4b9f-bc5a-0e3bcef9c56f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{021E385F-31AC-44DC-AD80-9ADB528DC174}">
   <ds:schemaRefs>
@@ -21217,6 +22023,24 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EDB03BF-0C37-4F11-B196-D49044127181}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="07fe17d8-c930-4881-be9b-3b241872ecf2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a516c34c-5f40-4b9f-bc5a-0e3bcef9c56f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0104D372-BA5B-4DD2-8ED7-FA9BFF6DAE56}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21234,22 +22058,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EDB03BF-0C37-4F11-B196-D49044127181}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="07fe17d8-c930-4881-be9b-3b241872ecf2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a516c34c-5f40-4b9f-bc5a-0e3bcef9c56f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>